<commit_message>
Refresh with latests copies
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FERCASTR\Documents\PaaS\OCI\DR\Hybrid\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546546CD-77F0-4E85-A38C-1E0BF182B666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7665" windowHeight="4245"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test44" sheetId="1" r:id="rId1"/>
+    <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
   <si>
     <t>Yes</t>
   </si>
@@ -346,9 +347,6 @@
     <t>oci-ohs-node_prefix/hostname</t>
   </si>
   <si>
-    <t>OCI OHS instances</t>
-  </si>
-  <si>
     <t>ON-PREM network</t>
   </si>
   <si>
@@ -385,18 +383,6 @@
     <t xml:space="preserve">Listen addresses </t>
   </si>
   <si>
-    <t>Shared config mountpoint</t>
-  </si>
-  <si>
-    <t>Shared runtime mountpoint</t>
-  </si>
-  <si>
-    <t>Products mountpoint</t>
-  </si>
-  <si>
-    <t>Private config mountpoint</t>
-  </si>
-  <si>
     <t>/u01/oracle/config</t>
   </si>
   <si>
@@ -406,12 +392,6 @@
     <t>/u01/oracle/runtime</t>
   </si>
   <si>
-    <t>/u02</t>
-  </si>
-  <si>
-    <t>prem-wls-mountpoints-config/path</t>
-  </si>
-  <si>
     <t>prem-wls-mountpoints-runtime/path</t>
   </si>
   <si>
@@ -481,21 +461,9 @@
     <t>oci-lbr-https_port/port</t>
   </si>
   <si>
-    <t>oci-lbr-admin_port/port</t>
-  </si>
-  <si>
     <t>LBR HTTPS port</t>
   </si>
   <si>
-    <t>LBR Admin port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OHS HTTP console port </t>
-  </si>
-  <si>
-    <t>oci-ohs-console_port/port</t>
-  </si>
-  <si>
     <t>OHS HTTP port</t>
   </si>
   <si>
@@ -511,155 +479,225 @@
     <t>oci-lbr-virtual_hostname_value/opt</t>
   </si>
   <si>
-    <t>LBR admin virtual hostname</t>
-  </si>
-  <si>
-    <t>wlsfrontendadmin.example.com</t>
+    <t>CA certificate path (leave blank for self-signed certs)</t>
+  </si>
+  <si>
+    <t>oci-network-ports-node_manager/port</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence/port</t>
+  </si>
+  <si>
+    <t>NodeManager port</t>
+  </si>
+  <si>
+    <t>Coherence port</t>
+  </si>
+  <si>
+    <t>10.1.1.0/24</t>
+  </si>
+  <si>
+    <t>10.1.1.32/27</t>
+  </si>
+  <si>
+    <t>10.1.1.64/26</t>
+  </si>
+  <si>
+    <t>10.1.1.128/26</t>
+  </si>
+  <si>
+    <t>10.1.1.192/26</t>
+  </si>
+  <si>
+    <t>prem-ohs-listen_addresses/str</t>
+  </si>
+  <si>
+    <t>PREM_OHS_LISTEN1</t>
+  </si>
+  <si>
+    <t>PREM_OHS_LISTEN2</t>
+  </si>
+  <si>
+    <t>webtierSubnet</t>
+  </si>
+  <si>
+    <t>midtierSubnet</t>
+  </si>
+  <si>
+    <t>dbtierSubnet</t>
+  </si>
+  <si>
+    <t>fsstierSubnet</t>
+  </si>
+  <si>
+    <t>DRmountTarget</t>
+  </si>
+  <si>
+    <t>wlsconfigFSS</t>
+  </si>
+  <si>
+    <t>wlsruntimeFSS</t>
+  </si>
+  <si>
+    <t>wlsproductsFSS</t>
+  </si>
+  <si>
+    <t>/export/wlsconfig</t>
+  </si>
+  <si>
+    <t>/export/wlsruntime</t>
+  </si>
+  <si>
+    <t>/export/wlsproducts</t>
+  </si>
+  <si>
+    <t>WlsNode</t>
+  </si>
+  <si>
+    <t>LBR</t>
+  </si>
+  <si>
+    <t>prem-wls-listen_addresses/fqdn</t>
+  </si>
+  <si>
+    <t>APPHOST1.example.com</t>
+  </si>
+  <si>
+    <t>APPHOST2.example.com</t>
+  </si>
+  <si>
+    <t>Listen addresses - FQDN</t>
+  </si>
+  <si>
+    <t>Products directory path</t>
+  </si>
+  <si>
+    <t>/u02/oracle/products</t>
+  </si>
+  <si>
+    <t>Private config directory path</t>
+  </si>
+  <si>
+    <t>/u02/oracle/config</t>
+  </si>
+  <si>
+    <t>prem-ohs-products_path/path</t>
+  </si>
+  <si>
+    <t>prem-ohs-config_path/path</t>
+  </si>
+  <si>
+    <t>/path/to/mycert.crt</t>
+  </si>
+  <si>
+    <t>/path/to/mycert.key</t>
+  </si>
+  <si>
+    <t>VCN-NAME</t>
+  </si>
+  <si>
+    <t>/path/to/private/key</t>
+  </si>
+  <si>
+    <t>/path/to/public/key</t>
+  </si>
+  <si>
+    <t>compartment_ocid</t>
+  </si>
+  <si>
+    <t>CA certificate passphrase (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>oci-lbr-virt_host_ohs_port/opt</t>
+  </si>
+  <si>
+    <t>oci-lbr-virt_host_hostname/opt</t>
+  </si>
+  <si>
+    <t>oci-lbr-virt_host_lbr_port/opt</t>
+  </si>
+  <si>
+    <t>OhsNode</t>
+  </si>
+  <si>
+    <t>needs custom input</t>
+  </si>
+  <si>
+    <t>default value  (column E) can be used</t>
+  </si>
+  <si>
+    <t>Custom value required?</t>
+  </si>
+  <si>
+    <t>Optional, provide only if explicitly required</t>
+  </si>
+  <si>
+    <t>/u02/xxx/yyy</t>
+  </si>
+  <si>
+    <t>We can DELETE this from the spreadsheet (now is always "oci")</t>
+  </si>
+  <si>
+    <t>We can DELETE this from the spreadsheet (now is always "No", because VCN must exist for the bastion)</t>
+  </si>
+  <si>
+    <t>Shared runtime mountpoint  (leave blank if not used)</t>
   </si>
   <si>
     <t>oci-lbr-admin_hostname_value/opt</t>
   </si>
   <si>
-    <t>CA certificate path (leave blank for self-signed certs)</t>
-  </si>
-  <si>
-    <t>oci-network-ports-node_manager/port</t>
-  </si>
-  <si>
-    <t>oci-network-ports-coherence/port</t>
-  </si>
-  <si>
-    <t>NodeManager port</t>
-  </si>
-  <si>
-    <t>Coherence port</t>
-  </si>
-  <si>
-    <t>10.1.1.0/24</t>
-  </si>
-  <si>
-    <t>10.1.1.32/27</t>
-  </si>
-  <si>
-    <t>10.1.1.64/26</t>
-  </si>
-  <si>
-    <t>10.1.1.128/26</t>
-  </si>
-  <si>
-    <t>10.1.1.192/26</t>
-  </si>
-  <si>
-    <t>prem-ohs-listen_addresses/str</t>
-  </si>
-  <si>
-    <t>PREM_OHS_LISTEN1</t>
-  </si>
-  <si>
-    <t>PREM_OHS_LISTEN2</t>
-  </si>
-  <si>
-    <t>webtierSubnet</t>
-  </si>
-  <si>
-    <t>midtierSubnet</t>
-  </si>
-  <si>
-    <t>dbtierSubnet</t>
-  </si>
-  <si>
-    <t>fsstierSubnet</t>
-  </si>
-  <si>
-    <t>DRmountTarget</t>
-  </si>
-  <si>
-    <t>wlsconfigFSS</t>
-  </si>
-  <si>
-    <t>wlsruntimeFSS</t>
-  </si>
-  <si>
-    <t>wlsproductsFSS</t>
-  </si>
-  <si>
-    <t>/export/wlsconfig</t>
-  </si>
-  <si>
-    <t>/export/wlsruntime</t>
-  </si>
-  <si>
-    <t>/export/wlsproducts</t>
-  </si>
-  <si>
-    <t>WlsNode</t>
-  </si>
-  <si>
-    <t>Ohs</t>
-  </si>
-  <si>
-    <t>LBR</t>
-  </si>
-  <si>
-    <t>prem-wls-listen_addresses/fqdn</t>
-  </si>
-  <si>
-    <t>APPHOST1.example.com</t>
-  </si>
-  <si>
-    <t>APPHOST2.example.com</t>
-  </si>
-  <si>
-    <t>Listen addresses - FQDN</t>
-  </si>
-  <si>
-    <t>Products directory path</t>
-  </si>
-  <si>
-    <t>/u02/oracle/products</t>
-  </si>
-  <si>
-    <t>Private config directory path</t>
-  </si>
-  <si>
-    <t>/u02/oracle/config</t>
-  </si>
-  <si>
-    <t>prem-ohs-products_path/path</t>
-  </si>
-  <si>
-    <t>prem-ohs-config_path/path</t>
-  </si>
-  <si>
-    <t>/path/to/mycert.crt</t>
-  </si>
-  <si>
-    <t>/path/to/mycert.key</t>
-  </si>
-  <si>
-    <t>VCN-NAME</t>
-  </si>
-  <si>
-    <t>/path/to/private/key</t>
-  </si>
-  <si>
-    <t>/path/to/public/key</t>
-  </si>
-  <si>
-    <t>compartment_ocid</t>
-  </si>
-  <si>
-    <t>CA certificate passphrase (leave blank if not used)</t>
+    <t>Shared config mountpoint       (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Products mountpoint                (if the products folder is in boot volume (mount point is /) then provide the products folder path)</t>
+  </si>
+  <si>
+    <t>prem-wls-mountpoints-config/opt</t>
+  </si>
+  <si>
+    <t>OCI OHS instances
+(clear all values if not used)</t>
+  </si>
+  <si>
+    <t>oci-lbr-admin_port/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-console_port/opt</t>
+  </si>
+  <si>
+    <t>Private config mountpoint     (if the private config folder is in boot volume (mount point is /) then provide the private config folder path)</t>
+  </si>
+  <si>
+    <t>OPTIONAL Advanced  Configuration</t>
+  </si>
+  <si>
+    <t>Internal virtual host-LBR Port  (e.g. for internal accesses like OWSM)                   (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-Frontend Name                                      (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-LBR Port                                                    (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-OHS HTTP port                                        (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-OHS HTTP port (e.g. for internal accesses like OWSM)        (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)      (leave blank if not used)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,8 +753,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -741,8 +786,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -750,12 +806,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -771,21 +867,55 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1063,209 +1193,245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:W101"/>
+  <dimension ref="A1:X104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:D66"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="124.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="48.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="1:24" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
         <v>89</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
       <c r="B3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="E3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
       <c r="B4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
         <v>93</v>
       </c>
-      <c r="D4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="E4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
       <c r="B5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
         <v>94</v>
       </c>
-      <c r="D5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="E5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
       <c r="B6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:24" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
         <v>52</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>135</v>
+      <c r="C8" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
       <c r="B9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="E9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
-        <v>131</v>
+      <c r="C10" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J10" s="6"/>
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>162</v>
+      </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="Q10" s="6"/>
+      <c r="P10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="X10" s="6"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>132</v>
+      <c r="C11" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
-      </c>
-      <c r="J11" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>163</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="Q11" s="6"/>
+      <c r="P11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>133</v>
+      <c r="C12" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>178</v>
-      </c>
-      <c r="J12" s="6"/>
+        <v>126</v>
+      </c>
+      <c r="E12" t="s">
+        <v>164</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -1279,19 +1445,22 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="X12" s="6"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>134</v>
+      <c r="C13" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" s="6"/>
+        <v>127</v>
+      </c>
+      <c r="E13" t="s">
+        <v>165</v>
+      </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -1305,19 +1474,22 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="X13" s="6"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -1331,19 +1503,22 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
@@ -1357,19 +1532,22 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="X15" s="6"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -1383,19 +1561,22 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" s="26"/>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -1409,19 +1590,22 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="X17" s="6"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" s="26"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>169</v>
-      </c>
-      <c r="J18" s="6"/>
+      <c r="E18" t="s">
+        <v>155</v>
+      </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1435,19 +1619,22 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="X18" s="6"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="D19" t="s">
-        <v>170</v>
-      </c>
-      <c r="J19" s="6"/>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1461,19 +1648,22 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="D20" t="s">
-        <v>171</v>
-      </c>
-      <c r="J20" s="6"/>
+      <c r="E20" t="s">
+        <v>157</v>
+      </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -1487,19 +1677,22 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="X20" s="6"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="D21" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21" s="6"/>
+      <c r="E21" t="s">
+        <v>158</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
@@ -1513,19 +1706,22 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="X21" s="6"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" t="s">
-        <v>130</v>
+      <c r="C22" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1539,19 +1735,22 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="X22" s="6"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>22</v>
       </c>
-      <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -1565,19 +1764,22 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="X23" s="6"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="8">
+      <c r="E24" s="8">
         <v>1521</v>
       </c>
-      <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1591,19 +1793,22 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="X24" s="6"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" t="s">
         <v>65</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>6200</v>
       </c>
-      <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -1617,19 +1822,22 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="X25" s="6"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
       <c r="B26" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" t="s">
-        <v>164</v>
-      </c>
-      <c r="D26">
+        <v>152</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D26" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26">
         <v>5556</v>
       </c>
-      <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -1643,19 +1851,22 @@
       <c r="U26" s="6"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="X26" s="6"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
       <c r="B27" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27">
+        <v>153</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27">
         <v>7574</v>
       </c>
-      <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -1669,703 +1880,887 @@
       <c r="U27" s="6"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D28" t="s">
         <v>66</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>7010</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>8001</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>8011</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>8021</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>9001</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="E29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" t="s">
         <v>84</v>
       </c>
-      <c r="D30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="E30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="D31" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="E31" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" t="s">
         <v>82</v>
       </c>
-      <c r="D32" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="E32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" t="s">
         <v>86</v>
       </c>
-      <c r="D33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="E33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" t="s">
         <v>87</v>
       </c>
-      <c r="D34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="E34" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D35" t="s">
         <v>79</v>
       </c>
-      <c r="D35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="E35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
       <c r="B37" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D37" t="s">
         <v>68</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="26"/>
       <c r="B38" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" t="s">
         <v>69</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="26"/>
       <c r="B39" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D39" t="s">
         <v>75</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="26"/>
       <c r="B40" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" t="s">
         <v>80</v>
       </c>
-      <c r="D40" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>105</v>
+      <c r="E40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D41" t="s">
         <v>100</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="25"/>
       <c r="B42" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" t="s">
         <v>101</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" t="s">
         <v>102</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
       <c r="B44" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D44" t="s">
         <v>103</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D45" t="s">
         <v>104</v>
       </c>
-      <c r="D45" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C46" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46">
-        <v>7001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+        <v>144</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>133</v>
+      </c>
       <c r="B47" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" t="s">
-        <v>156</v>
-      </c>
-      <c r="D47">
-        <v>7777</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="26"/>
+      <c r="B48" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="C48" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="26"/>
+      <c r="B49" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="26"/>
+      <c r="B50" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" t="s">
         <v>136</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E50" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="26"/>
+      <c r="B51" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="26"/>
+      <c r="B52" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D52" t="s">
         <v>137</v>
       </c>
-      <c r="D48" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="5" t="s">
+      <c r="E52" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="26"/>
+      <c r="B53" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="26"/>
+      <c r="B54" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" t="s">
         <v>147</v>
       </c>
-      <c r="C49" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" t="s">
-        <v>139</v>
-      </c>
-      <c r="D50">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="26"/>
+      <c r="B55" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D51" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="5" t="s">
+      <c r="C55" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D55" t="s">
         <v>142</v>
       </c>
-      <c r="C53" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="5" t="s">
+      <c r="E55">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="26"/>
+      <c r="B58" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="26"/>
+      <c r="B59" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" t="s">
+        <v>175</v>
+      </c>
+      <c r="E59" t="s">
+        <v>176</v>
+      </c>
+      <c r="F59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="26"/>
+      <c r="B60" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="26"/>
+      <c r="B61" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" t="s">
+        <v>120</v>
+      </c>
+      <c r="E61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="26"/>
+      <c r="B62" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C54" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C55" t="s">
-        <v>159</v>
-      </c>
-      <c r="D55" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C56" t="s">
-        <v>162</v>
-      </c>
-      <c r="D56" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C57" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C58" t="s">
-        <v>150</v>
-      </c>
-      <c r="D58">
-        <v>7001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" t="s">
-        <v>109</v>
-      </c>
-      <c r="D60">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C62" t="s">
-        <v>190</v>
+      <c r="C62" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="E62" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="26"/>
       <c r="B63" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C63" t="s">
-        <v>126</v>
+        <v>211</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="E63" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="25" t="s">
+        <v>107</v>
+      </c>
       <c r="B64" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" t="s">
-        <v>127</v>
+        <v>114</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
+        <v>110</v>
+      </c>
+      <c r="E64">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="25"/>
       <c r="B65" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+        <v>111</v>
+      </c>
+      <c r="E65">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="25"/>
       <c r="B66" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" t="s">
-        <v>129</v>
+        <v>116</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="D66" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>108</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E66" t="s">
+        <v>160</v>
+      </c>
+      <c r="F66" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="25"/>
       <c r="B67" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C67" t="s">
-        <v>111</v>
-      </c>
-      <c r="D67">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+        <v>179</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" t="s">
+        <v>183</v>
+      </c>
+      <c r="E67" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="25"/>
       <c r="B68" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" t="s">
-        <v>112</v>
-      </c>
-      <c r="D68">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" t="s">
-        <v>173</v>
+        <v>181</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D68" t="s">
+        <v>184</v>
+      </c>
+      <c r="E68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>199</v>
       </c>
       <c r="D69" t="s">
-        <v>174</v>
-      </c>
-      <c r="E69" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="24"/>
       <c r="B70" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D70" t="s">
         <v>194</v>
       </c>
-      <c r="C70" t="s">
-        <v>198</v>
-      </c>
-      <c r="D70" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="24"/>
       <c r="B71" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C71" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="19" t="s">
         <v>199</v>
       </c>
       <c r="D71" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="24"/>
+      <c r="B72" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="24"/>
+      <c r="B73" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="24"/>
+      <c r="B74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="B75" s="4"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
+    <row r="87" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-    </row>
-    <row r="86" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="s">
+      <c r="C87" s="22"/>
+    </row>
+    <row r="88" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="10"/>
+      <c r="C88" s="22"/>
+    </row>
+    <row r="89" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="s">
+      <c r="C89" s="22"/>
+    </row>
+    <row r="90" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
-    </row>
-    <row r="89" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+      <c r="C90" s="22"/>
+    </row>
+    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+      <c r="C91" s="22"/>
+    </row>
+    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
-    </row>
-    <row r="92" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-    </row>
-    <row r="93" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+      <c r="C93" s="22"/>
+    </row>
+    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="10"/>
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="10"/>
+      <c r="C95" s="22"/>
+    </row>
+    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
+      <c r="C97" s="22"/>
+    </row>
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-    </row>
-    <row r="99" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
-    </row>
-    <row r="100" spans="1:1" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="10"/>
+      <c r="C101" s="22"/>
+    </row>
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="10"/>
+      <c r="C102" s="22"/>
+    </row>
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
+      <c r="C103" s="22"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="10" t="s">
         <v>91</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A67:A69"/>
+  <mergeCells count="9">
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="F1:L1"/>
     <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A48:A58"/>
-    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="A41:A46"/>
     <mergeCell ref="A2:A28"/>
   </mergeCells>
-  <dataValidations count="10">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B29"/>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23">
+  <dataValidations count="11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B29" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D6:D7 D15:D17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22 E6:E7 E15:E17" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D14">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D36 D41">
-      <formula1>$A$89:$A$90</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E36 E41" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>$A$92:$A$93</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="D37:D39 D42:D44">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E42:E43" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1>$A$100:$A$101</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
+      <formula1>$A$103:$A$104</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D49:D50">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E48:E49" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
       <formula2>4800</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E44" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update to WLS_HYDR framework per latest features
This is grabbing baseline from orahub as of November 6rh 2024
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FERCASTR\Documents\PaaS\OCI\DR\Hybrid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546546CD-77F0-4E85-A38C-1E0BF182B666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5515ACC2-1EE6-4AB4-86BC-A25A734C0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="229">
   <si>
     <t>Yes</t>
   </si>
@@ -145,12 +146,6 @@
     <t>Oracle WebLogic Suite UCM Image</t>
   </si>
   <si>
-    <t>7.9</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
     <t>Weblogic OS version</t>
   </si>
   <si>
@@ -179,12 +174,6 @@
     <t>Weblogic memory</t>
   </si>
   <si>
-    <t>VCN name</t>
-  </si>
-  <si>
-    <t>VCN CIDR</t>
-  </si>
-  <si>
     <t>Create VCN?</t>
   </si>
   <si>
@@ -335,51 +324,12 @@
     <t>oci-ohs-os_version/opt</t>
   </si>
   <si>
-    <t>oci-ohs-ocpu/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-memory/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-nodes_count/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-node_prefix/hostname</t>
-  </si>
-  <si>
     <t>ON-PREM network</t>
   </si>
   <si>
     <t>ON-PREM WLS</t>
   </si>
   <si>
-    <t>ON-PREM OHS</t>
-  </si>
-  <si>
-    <t>prem-wls-oinstall_gid/int</t>
-  </si>
-  <si>
-    <t>prem-wls-oracle_uid/int</t>
-  </si>
-  <si>
-    <t>prem-ohs-oinstall_gid/int</t>
-  </si>
-  <si>
-    <t>prem-ohs-oracle_uid/int</t>
-  </si>
-  <si>
-    <t>WLS oinstall group ID</t>
-  </si>
-  <si>
-    <t>WLS oracle user ID</t>
-  </si>
-  <si>
-    <t>OHS oinstall group ID</t>
-  </si>
-  <si>
-    <t>OHS oracle user ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listen addresses </t>
   </si>
   <si>
@@ -458,18 +408,12 @@
     <t>LBR maximum bandwidth (10-4800)</t>
   </si>
   <si>
-    <t>oci-lbr-https_port/port</t>
-  </si>
-  <si>
     <t>LBR HTTPS port</t>
   </si>
   <si>
     <t>OHS HTTP port</t>
   </si>
   <si>
-    <t>oci-ohs-http_port/port</t>
-  </si>
-  <si>
     <t>LBR virtual hostname</t>
   </si>
   <si>
@@ -509,9 +453,6 @@
     <t>10.1.1.192/26</t>
   </si>
   <si>
-    <t>prem-ohs-listen_addresses/str</t>
-  </si>
-  <si>
     <t>PREM_OHS_LISTEN1</t>
   </si>
   <si>
@@ -581,12 +522,6 @@
     <t>/u02/oracle/config</t>
   </si>
   <si>
-    <t>prem-ohs-products_path/path</t>
-  </si>
-  <si>
-    <t>prem-ohs-config_path/path</t>
-  </si>
-  <si>
     <t>/path/to/mycert.crt</t>
   </si>
   <si>
@@ -629,16 +564,7 @@
     <t>Custom value required?</t>
   </si>
   <si>
-    <t>Optional, provide only if explicitly required</t>
-  </si>
-  <si>
-    <t>/u02/xxx/yyy</t>
-  </si>
-  <si>
     <t>We can DELETE this from the spreadsheet (now is always "oci")</t>
-  </si>
-  <si>
-    <t>We can DELETE this from the spreadsheet (now is always "No", because VCN must exist for the bastion)</t>
   </si>
   <si>
     <t>Shared runtime mountpoint  (leave blank if not used)</t>
@@ -688,6 +614,112 @@
   </si>
   <si>
     <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)      (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>prem-ohs-listen_addresses/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-products_path/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-config_path/opt</t>
+  </si>
+  <si>
+    <t>ON-PREM OHS
+(clear all values if not used)</t>
+  </si>
+  <si>
+    <t>oci-ohs-ocpu/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-memory/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-nodes_count/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-node_prefix/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-http_port/opt</t>
+  </si>
+  <si>
+    <t>oci-lbr-https_port/opt</t>
+  </si>
+  <si>
+    <t>WLS owner OS user name</t>
+  </si>
+  <si>
+    <t>WLS owner OS group name</t>
+  </si>
+  <si>
+    <t>oracle</t>
+  </si>
+  <si>
+    <t>oinstall</t>
+  </si>
+  <si>
+    <t>WLS owner OS group ID</t>
+  </si>
+  <si>
+    <t>WLS owner OS user ID</t>
+  </si>
+  <si>
+    <t>prem-wls-group_gid/int</t>
+  </si>
+  <si>
+    <t>prem-wls-user_uid/int</t>
+  </si>
+  <si>
+    <t>prem-wls-user_name/name</t>
+  </si>
+  <si>
+    <t>prem-wls-group_name/name</t>
+  </si>
+  <si>
+    <t>prem-ohs-user_uid/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-group_gid/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-user_name/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-group_name/opt</t>
+  </si>
+  <si>
+    <t>OSH owner OS user name</t>
+  </si>
+  <si>
+    <t>OSH owner OS user ID</t>
+  </si>
+  <si>
+    <t>OSH owner OS group ID</t>
+  </si>
+  <si>
+    <t>OSH owner OS group name</t>
+  </si>
+  <si>
+    <t>/u02</t>
+  </si>
+  <si>
+    <t>Optional - provide only if explicitly required</t>
+  </si>
+  <si>
+    <t>We can DELETE this from the spreadsheet (now is always "No" because VCN must exist for the bastion)</t>
+  </si>
+  <si>
+    <t>Existing VCN CIDR</t>
+  </si>
+  <si>
+    <t>Existing VCN Name</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -695,7 +727,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -798,7 +830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -821,37 +853,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,16 +905,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1197,26 +1199,26 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X104"/>
+  <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="124.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="121.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1224,157 +1226,157 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-    </row>
-    <row r="2" spans="1:24" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C5" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="5" t="s">
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C6" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
       <c r="B8" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
       <c r="E9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1390,19 +1392,19 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1418,19 +1420,19 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1447,19 +1449,19 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1476,16 +1478,16 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1505,16 +1507,16 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -1534,16 +1536,16 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -1563,16 +1565,16 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1592,19 +1594,19 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1621,19 +1623,19 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1650,19 +1652,19 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1679,19 +1681,19 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1708,16 +1710,16 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1737,16 +1739,16 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E23" s="7">
         <v>22</v>
@@ -1766,16 +1768,16 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E24" s="8">
         <v>1521</v>
@@ -1795,16 +1797,16 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>6200</v>
@@ -1824,16 +1826,16 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1853,16 +1855,16 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
       <c r="B27" s="5" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1882,16 +1884,16 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1909,829 +1911,903 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
       <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
       <c r="B35" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
       <c r="B38" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E38">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
       <c r="B39" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
-        <v>208</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>183</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
       <c r="B43" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="E43">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>200</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="E45" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
       <c r="B46" s="5" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="E46">
         <v>7777</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
-        <v>133</v>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
       <c r="B49" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E49">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
       <c r="B51" s="5" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
       <c r="B52" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
       <c r="B53" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
       <c r="B54" s="5" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="26"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
       <c r="B55" s="5" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="E55">
         <v>443</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
-        <v>106</v>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E57">
+        <v>212</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" t="s">
+        <v>211</v>
+      </c>
+      <c r="E58" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" t="s">
+        <v>213</v>
+      </c>
+      <c r="E59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60">
         <v>1002</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D58" t="s">
-        <v>109</v>
-      </c>
-      <c r="E58">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" t="s">
+        <v>155</v>
+      </c>
+      <c r="E61" t="s">
+        <v>156</v>
+      </c>
+      <c r="F61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" t="s">
+        <v>105</v>
+      </c>
+      <c r="E65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E66" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+      <c r="B67" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" t="s">
+        <v>214</v>
+      </c>
+      <c r="E67">
         <v>1001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D59" t="s">
-        <v>175</v>
-      </c>
-      <c r="E59" t="s">
-        <v>176</v>
-      </c>
-      <c r="F59" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D60" t="s">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" t="s">
         <v>207</v>
       </c>
-      <c r="E60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D61" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" t="s">
-        <v>121</v>
-      </c>
-      <c r="E62" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D63" t="s">
-        <v>122</v>
-      </c>
-      <c r="E63" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
+      <c r="B69" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" t="s">
+        <v>215</v>
+      </c>
+      <c r="E69">
         <v>1002</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="25"/>
-      <c r="B65" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D65" t="s">
-        <v>111</v>
-      </c>
-      <c r="E65">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="25"/>
-      <c r="B66" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D66" t="s">
-        <v>159</v>
-      </c>
-      <c r="E66" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="25"/>
-      <c r="B67" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" t="s">
-        <v>183</v>
-      </c>
-      <c r="E67" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="25"/>
-      <c r="B68" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D68" t="s">
-        <v>184</v>
-      </c>
-      <c r="E68" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D69" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="24"/>
       <c r="B70" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>199</v>
+        <v>99</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D70" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>140</v>
+      </c>
+      <c r="F70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="24"/>
       <c r="B71" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>199</v>
+        <v>159</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D71" t="s">
+        <v>195</v>
+      </c>
+      <c r="E71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
+      <c r="B72" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D72" t="s">
+        <v>196</v>
+      </c>
+      <c r="E72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="24"/>
-      <c r="B72" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="24"/>
-      <c r="B73" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D73" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="24"/>
-      <c r="B74" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D74" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
+      <c r="C75" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+      <c r="B77" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+      <c r="B78" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D78" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="B79" s="4"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
+      <c r="B90" s="9"/>
+    </row>
+    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C87" s="22"/>
-    </row>
-    <row r="88" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10"/>
-      <c r="C88" s="22"/>
-    </row>
-    <row r="89" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="s">
+      <c r="C91" s="22"/>
+    </row>
+    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="22"/>
-    </row>
-    <row r="90" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
+      <c r="C93" s="22"/>
+    </row>
+    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C90" s="22"/>
-    </row>
-    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10"/>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C93" s="22"/>
-    </row>
-    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="10"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
+    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" s="22"/>
+    </row>
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10"/>
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C101" s="22"/>
+    </row>
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C96" s="22"/>
-    </row>
-    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
+      <c r="C102" s="22"/>
+    </row>
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C97" s="22"/>
-    </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
+      <c r="C103" s="22"/>
+    </row>
+    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C98" s="22"/>
-    </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C99" s="22"/>
-    </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C100" s="22"/>
-    </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="10"/>
-      <c r="C101" s="22"/>
-    </row>
-    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="10"/>
-      <c r="C102" s="22"/>
-    </row>
-    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C103" s="22"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="C104" s="22"/>
+    </row>
+    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="10"/>
+      <c r="C105" s="22"/>
+    </row>
+    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="10"/>
+      <c r="C106" s="22"/>
+    </row>
+    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="22"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="9"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A73:A78"/>
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="A2:A28"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="A66:A72"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -2747,13 +2823,13 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E36 E41" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$92:$A$93</formula1>
+      <formula1>$A$96:$A$97</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E42:E43" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$103:$A$104</formula1>
+      <formula1>$A$107:$A$108</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E48:E49" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
@@ -2765,5 +2841,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A96:A97 E36 E41" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to WLS_HYDR framework per latest features (#95)
This is grabbing baseline from orahub as of November 6rh 2024
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FERCASTR\Documents\PaaS\OCI\DR\Hybrid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546546CD-77F0-4E85-A38C-1E0BF182B666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5515ACC2-1EE6-4AB4-86BC-A25A734C0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="229">
   <si>
     <t>Yes</t>
   </si>
@@ -145,12 +146,6 @@
     <t>Oracle WebLogic Suite UCM Image</t>
   </si>
   <si>
-    <t>7.9</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
     <t>Weblogic OS version</t>
   </si>
   <si>
@@ -179,12 +174,6 @@
     <t>Weblogic memory</t>
   </si>
   <si>
-    <t>VCN name</t>
-  </si>
-  <si>
-    <t>VCN CIDR</t>
-  </si>
-  <si>
     <t>Create VCN?</t>
   </si>
   <si>
@@ -335,51 +324,12 @@
     <t>oci-ohs-os_version/opt</t>
   </si>
   <si>
-    <t>oci-ohs-ocpu/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-memory/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-nodes_count/int</t>
-  </si>
-  <si>
-    <t>oci-ohs-node_prefix/hostname</t>
-  </si>
-  <si>
     <t>ON-PREM network</t>
   </si>
   <si>
     <t>ON-PREM WLS</t>
   </si>
   <si>
-    <t>ON-PREM OHS</t>
-  </si>
-  <si>
-    <t>prem-wls-oinstall_gid/int</t>
-  </si>
-  <si>
-    <t>prem-wls-oracle_uid/int</t>
-  </si>
-  <si>
-    <t>prem-ohs-oinstall_gid/int</t>
-  </si>
-  <si>
-    <t>prem-ohs-oracle_uid/int</t>
-  </si>
-  <si>
-    <t>WLS oinstall group ID</t>
-  </si>
-  <si>
-    <t>WLS oracle user ID</t>
-  </si>
-  <si>
-    <t>OHS oinstall group ID</t>
-  </si>
-  <si>
-    <t>OHS oracle user ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listen addresses </t>
   </si>
   <si>
@@ -458,18 +408,12 @@
     <t>LBR maximum bandwidth (10-4800)</t>
   </si>
   <si>
-    <t>oci-lbr-https_port/port</t>
-  </si>
-  <si>
     <t>LBR HTTPS port</t>
   </si>
   <si>
     <t>OHS HTTP port</t>
   </si>
   <si>
-    <t>oci-ohs-http_port/port</t>
-  </si>
-  <si>
     <t>LBR virtual hostname</t>
   </si>
   <si>
@@ -509,9 +453,6 @@
     <t>10.1.1.192/26</t>
   </si>
   <si>
-    <t>prem-ohs-listen_addresses/str</t>
-  </si>
-  <si>
     <t>PREM_OHS_LISTEN1</t>
   </si>
   <si>
@@ -581,12 +522,6 @@
     <t>/u02/oracle/config</t>
   </si>
   <si>
-    <t>prem-ohs-products_path/path</t>
-  </si>
-  <si>
-    <t>prem-ohs-config_path/path</t>
-  </si>
-  <si>
     <t>/path/to/mycert.crt</t>
   </si>
   <si>
@@ -629,16 +564,7 @@
     <t>Custom value required?</t>
   </si>
   <si>
-    <t>Optional, provide only if explicitly required</t>
-  </si>
-  <si>
-    <t>/u02/xxx/yyy</t>
-  </si>
-  <si>
     <t>We can DELETE this from the spreadsheet (now is always "oci")</t>
-  </si>
-  <si>
-    <t>We can DELETE this from the spreadsheet (now is always "No", because VCN must exist for the bastion)</t>
   </si>
   <si>
     <t>Shared runtime mountpoint  (leave blank if not used)</t>
@@ -688,6 +614,112 @@
   </si>
   <si>
     <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)      (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>prem-ohs-listen_addresses/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-products_path/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-config_path/opt</t>
+  </si>
+  <si>
+    <t>ON-PREM OHS
+(clear all values if not used)</t>
+  </si>
+  <si>
+    <t>oci-ohs-ocpu/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-memory/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-nodes_count/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-node_prefix/opt</t>
+  </si>
+  <si>
+    <t>oci-ohs-http_port/opt</t>
+  </si>
+  <si>
+    <t>oci-lbr-https_port/opt</t>
+  </si>
+  <si>
+    <t>WLS owner OS user name</t>
+  </si>
+  <si>
+    <t>WLS owner OS group name</t>
+  </si>
+  <si>
+    <t>oracle</t>
+  </si>
+  <si>
+    <t>oinstall</t>
+  </si>
+  <si>
+    <t>WLS owner OS group ID</t>
+  </si>
+  <si>
+    <t>WLS owner OS user ID</t>
+  </si>
+  <si>
+    <t>prem-wls-group_gid/int</t>
+  </si>
+  <si>
+    <t>prem-wls-user_uid/int</t>
+  </si>
+  <si>
+    <t>prem-wls-user_name/name</t>
+  </si>
+  <si>
+    <t>prem-wls-group_name/name</t>
+  </si>
+  <si>
+    <t>prem-ohs-user_uid/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-group_gid/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-user_name/opt</t>
+  </si>
+  <si>
+    <t>prem-ohs-group_name/opt</t>
+  </si>
+  <si>
+    <t>OSH owner OS user name</t>
+  </si>
+  <si>
+    <t>OSH owner OS user ID</t>
+  </si>
+  <si>
+    <t>OSH owner OS group ID</t>
+  </si>
+  <si>
+    <t>OSH owner OS group name</t>
+  </si>
+  <si>
+    <t>/u02</t>
+  </si>
+  <si>
+    <t>Optional - provide only if explicitly required</t>
+  </si>
+  <si>
+    <t>We can DELETE this from the spreadsheet (now is always "No" because VCN must exist for the bastion)</t>
+  </si>
+  <si>
+    <t>Existing VCN CIDR</t>
+  </si>
+  <si>
+    <t>Existing VCN Name</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -695,7 +727,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -798,7 +830,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -821,37 +853,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -897,16 +905,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1197,26 +1199,26 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X104"/>
+  <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="124.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="49.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="121.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1224,157 +1226,157 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-    </row>
-    <row r="2" spans="1:24" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C5" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="5" t="s">
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C6" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
       <c r="B7" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
       <c r="B8" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
       <c r="E9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1390,19 +1392,19 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1418,19 +1420,19 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1447,19 +1449,19 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1476,16 +1478,16 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1505,16 +1507,16 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -1534,16 +1536,16 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -1563,16 +1565,16 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1592,19 +1594,19 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1621,19 +1623,19 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1650,19 +1652,19 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1679,19 +1681,19 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1708,16 +1710,16 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1737,16 +1739,16 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E23" s="7">
         <v>22</v>
@@ -1766,16 +1768,16 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E24" s="8">
         <v>1521</v>
@@ -1795,16 +1797,16 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>6200</v>
@@ -1824,16 +1826,16 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1853,16 +1855,16 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
       <c r="B27" s="5" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1882,16 +1884,16 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1909,829 +1911,903 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
       <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
       <c r="B34" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
       <c r="B35" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>44</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
       <c r="B38" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E38">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
       <c r="B39" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
-        <v>208</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>183</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>198</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
       <c r="B43" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D43" t="s">
-        <v>102</v>
+        <v>199</v>
       </c>
       <c r="E43">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>200</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>104</v>
+        <v>201</v>
       </c>
       <c r="E45" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
       <c r="B46" s="5" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="E46">
         <v>7777</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
-        <v>133</v>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E48">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
       <c r="B49" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E49">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
       <c r="B50" s="5" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
       <c r="B51" s="5" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
       <c r="B52" s="5" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
       <c r="B53" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
       <c r="B54" s="5" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="26"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
       <c r="B55" s="5" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="E55">
         <v>443</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B56" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
-        <v>106</v>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E57">
+        <v>212</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" t="s">
+        <v>211</v>
+      </c>
+      <c r="E58" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" t="s">
+        <v>213</v>
+      </c>
+      <c r="E59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60">
         <v>1002</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D58" t="s">
-        <v>109</v>
-      </c>
-      <c r="E58">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" t="s">
+        <v>155</v>
+      </c>
+      <c r="E61" t="s">
+        <v>156</v>
+      </c>
+      <c r="F61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" t="s">
+        <v>105</v>
+      </c>
+      <c r="E65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D66" t="s">
+        <v>216</v>
+      </c>
+      <c r="E66" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+      <c r="B67" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" t="s">
+        <v>214</v>
+      </c>
+      <c r="E67">
         <v>1001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D59" t="s">
-        <v>175</v>
-      </c>
-      <c r="E59" t="s">
-        <v>176</v>
-      </c>
-      <c r="F59" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D60" t="s">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" t="s">
         <v>207</v>
       </c>
-      <c r="E60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D61" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D62" t="s">
-        <v>121</v>
-      </c>
-      <c r="E62" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D63" t="s">
-        <v>122</v>
-      </c>
-      <c r="E63" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D64" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
+      <c r="B69" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" t="s">
+        <v>215</v>
+      </c>
+      <c r="E69">
         <v>1002</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="25"/>
-      <c r="B65" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D65" t="s">
-        <v>111</v>
-      </c>
-      <c r="E65">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="25"/>
-      <c r="B66" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D66" t="s">
-        <v>159</v>
-      </c>
-      <c r="E66" t="s">
-        <v>160</v>
-      </c>
-      <c r="F66" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="25"/>
-      <c r="B67" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" t="s">
-        <v>183</v>
-      </c>
-      <c r="E67" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="25"/>
-      <c r="B68" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D68" t="s">
-        <v>184</v>
-      </c>
-      <c r="E68" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D69" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="24"/>
       <c r="B70" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>199</v>
+        <v>99</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D70" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>140</v>
+      </c>
+      <c r="F70" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="24"/>
       <c r="B71" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>199</v>
+        <v>159</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D71" t="s">
+        <v>195</v>
+      </c>
+      <c r="E71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
+      <c r="B72" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D72" t="s">
+        <v>196</v>
+      </c>
+      <c r="E72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="24"/>
-      <c r="B72" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="24"/>
-      <c r="B73" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D73" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="24"/>
-      <c r="B74" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D74" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
+      <c r="C75" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+      <c r="B77" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+      <c r="B78" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D78" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="B79" s="4"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
+      <c r="B90" s="9"/>
+    </row>
+    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C87" s="22"/>
-    </row>
-    <row r="88" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10"/>
-      <c r="C88" s="22"/>
-    </row>
-    <row r="89" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="s">
+      <c r="C91" s="22"/>
+    </row>
+    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="C92" s="22"/>
+    </row>
+    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="22"/>
-    </row>
-    <row r="90" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
+      <c r="C93" s="22"/>
+    </row>
+    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C90" s="22"/>
-    </row>
-    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="10"/>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C93" s="22"/>
-    </row>
-    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="10"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
+    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" s="22"/>
+    </row>
+    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" s="22"/>
+    </row>
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10"/>
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C101" s="22"/>
+    </row>
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C96" s="22"/>
-    </row>
-    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
+      <c r="C102" s="22"/>
+    </row>
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C97" s="22"/>
-    </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
+      <c r="C103" s="22"/>
+    </row>
+    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C98" s="22"/>
-    </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C99" s="22"/>
-    </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C100" s="22"/>
-    </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="10"/>
-      <c r="C101" s="22"/>
-    </row>
-    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="10"/>
-      <c r="C102" s="22"/>
-    </row>
-    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C103" s="22"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="s">
-        <v>91</v>
-      </c>
+      <c r="C104" s="22"/>
+    </row>
+    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="10"/>
+      <c r="C105" s="22"/>
+    </row>
+    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="10"/>
+      <c r="C106" s="22"/>
+    </row>
+    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="22"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="9"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A69:A74"/>
-    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A73:A78"/>
     <mergeCell ref="A47:A55"/>
     <mergeCell ref="A29:A35"/>
     <mergeCell ref="F1:L1"/>
     <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A57:A63"/>
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="A2:A28"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="A66:A72"/>
   </mergeCells>
   <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -2747,13 +2823,13 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E36 E41" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$92:$A$93</formula1>
+      <formula1>$A$96:$A$97</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E42:E43" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$103:$A$104</formula1>
+      <formula1>$A$107:$A$108</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E48:E49" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
@@ -2765,5 +2841,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A96:A97 E36 E41" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of readm and push to Github fof latest Orahub Changes
Update per latest terminology and ERs per feb 20th 2025
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5515ACC2-1EE6-4AB4-86BC-A25A734C0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C92B609-4F14-45CC-BBA9-A40D42493029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7050" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="235">
   <si>
     <t>Yes</t>
   </si>
@@ -219,9 +218,6 @@
     <t>oci-network-ports-ons/port</t>
   </si>
   <si>
-    <t>oci-network-ports-wlsservers/port</t>
-  </si>
-  <si>
     <t>oci-wls-os_version/opt</t>
   </si>
   <si>
@@ -598,24 +594,6 @@
     <t>OPTIONAL Advanced  Configuration</t>
   </si>
   <si>
-    <t>Internal virtual host-LBR Port  (e.g. for internal accesses like OWSM)                   (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-Frontend Name                                      (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-LBR Port                                                    (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-OHS HTTP port                                        (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Internal virtual host-OHS HTTP port (e.g. for internal accesses like OWSM)        (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)      (leave blank if not used)</t>
-  </si>
-  <si>
     <t>prem-ohs-listen_addresses/opt</t>
   </si>
   <si>
@@ -720,6 +698,45 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>WLS administration ports</t>
+  </si>
+  <si>
+    <t>WLS channels listen ports</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsadmin/port</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsservers/opt</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlschannels/opt</t>
+  </si>
+  <si>
+    <t>prem-wls-vipaddress/opt</t>
+  </si>
+  <si>
+    <t>If the Admin Server listens in a Virtual IP address, provide the virtual FQDN hostname value (e.g. asvip.example.com)    (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-OHS HTTP port                                                                                                                                 (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-Frontend Name                                                                                                                               (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-OHS HTTP port (e.g. for internal accesses like OWSM)                                                                                              (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-LBR Port  (e.g. for internal accesses like OWSM)                                                                                                          (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)                                                                                            (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-LBR Port                                                                                                                                              (leave blank if not used)</t>
   </si>
 </sst>
 </file>
@@ -727,7 +744,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -856,10 +873,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -904,6 +921,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1199,16 +1219,16 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X110"/>
+  <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="121.42578125" customWidth="1"/>
+    <col min="2" max="2" width="128.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
     <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
@@ -1226,106 +1246,106 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-    </row>
-    <row r="2" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C4" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
         <v>72</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -1335,48 +1355,48 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1393,18 +1413,18 @@
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1421,18 +1441,18 @@
       <c r="X11" s="6"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1450,18 +1470,18 @@
       <c r="X12" s="6"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1479,12 +1499,12 @@
       <c r="X13" s="6"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
@@ -1508,12 +1528,12 @@
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -1537,12 +1557,12 @@
       <c r="X15" s="6"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1566,12 +1586,12 @@
       <c r="X16" s="6"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -1595,18 +1615,18 @@
       <c r="X17" s="6"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1624,18 +1644,18 @@
       <c r="X18" s="6"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D19" t="s">
         <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1653,18 +1673,18 @@
       <c r="X19" s="6"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1682,18 +1702,18 @@
       <c r="X20" s="6"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1711,15 +1731,15 @@
       <c r="X21" s="6"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1740,12 +1760,12 @@
       <c r="X22" s="6"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1769,12 +1789,12 @@
       <c r="X23" s="6"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
@@ -1798,12 +1818,12 @@
       <c r="X24" s="6"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
@@ -1827,15 +1847,15 @@
       <c r="X25" s="6"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1856,15 +1876,15 @@
       <c r="X26" s="6"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1885,15 +1905,15 @@
       <c r="X27" s="6"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>225</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1911,823 +1931,843 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>28</v>
-      </c>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>175</v>
+        <v>223</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>216</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C32" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" t="s">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" t="s">
         <v>81</v>
       </c>
-      <c r="E31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" t="s">
         <v>82</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" t="s">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C38" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" t="s">
         <v>63</v>
       </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" t="s">
         <v>64</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38">
+      <c r="E40">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="5" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39">
+      <c r="E41">
         <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="25"/>
+      <c r="B44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C45" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" t="s">
+        <v>192</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
+      <c r="B46" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="B50" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+      <c r="B52" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
+      <c r="B53" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="24"/>
+      <c r="B54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="B55" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
+      <c r="B56" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
+      <c r="B57" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D57" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" t="s">
+        <v>205</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="24"/>
+      <c r="B60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" t="s">
+        <v>204</v>
+      </c>
+      <c r="E60" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+      <c r="B61" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" t="s">
-        <v>199</v>
-      </c>
-      <c r="E43">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C61" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" t="s">
+        <v>206</v>
+      </c>
+      <c r="E61" t="s">
         <v>200</v>
       </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="24"/>
+      <c r="B62" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" t="s">
-        <v>202</v>
-      </c>
-      <c r="E46">
-        <v>7777</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" t="s">
-        <v>113</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="C62" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+      <c r="B63" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49">
+      <c r="E63" t="s">
+        <v>155</v>
+      </c>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="24"/>
+      <c r="B64" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="24"/>
+      <c r="B65" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D65" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24"/>
+      <c r="B66" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E52" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" t="s">
-        <v>203</v>
-      </c>
-      <c r="E55">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" t="s">
-        <v>212</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" t="s">
-        <v>211</v>
-      </c>
-      <c r="E58" s="14">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D59" t="s">
-        <v>213</v>
-      </c>
-      <c r="E59" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" t="s">
-        <v>210</v>
-      </c>
-      <c r="E60">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D61" t="s">
-        <v>155</v>
-      </c>
-      <c r="E61" t="s">
-        <v>156</v>
-      </c>
-      <c r="F61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D62" t="s">
-        <v>182</v>
-      </c>
-      <c r="E62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" t="s">
-        <v>103</v>
-      </c>
-      <c r="E63" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D64" t="s">
-        <v>104</v>
-      </c>
-      <c r="E64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D65" t="s">
-        <v>105</v>
-      </c>
-      <c r="E65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D66" t="s">
-        <v>216</v>
-      </c>
-      <c r="E66" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D67" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" t="s">
+        <v>209</v>
+      </c>
+      <c r="E68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="25"/>
+      <c r="B69" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="25"/>
+      <c r="B70" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E67">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
-      <c r="B68" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D68" t="s">
-        <v>217</v>
-      </c>
-      <c r="E68" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="24"/>
-      <c r="B69" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" t="s">
-        <v>215</v>
-      </c>
-      <c r="E69">
+      <c r="C70" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="25"/>
+      <c r="B71" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D71" t="s">
+        <v>208</v>
+      </c>
+      <c r="E71">
         <v>1002</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
-      <c r="B70" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D70" t="s">
-        <v>194</v>
-      </c>
-      <c r="E70" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="25"/>
+      <c r="B72" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D72" t="s">
+        <v>187</v>
+      </c>
+      <c r="E72" t="s">
+        <v>139</v>
+      </c>
+      <c r="F72" t="s">
         <v>140</v>
       </c>
-      <c r="F70" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
-      <c r="B71" s="5" t="s">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="25"/>
+      <c r="B73" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D73" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" t="s">
         <v>159</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D71" t="s">
-        <v>195</v>
-      </c>
-      <c r="E71" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="25"/>
+      <c r="B74" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
-      <c r="B72" s="5" t="s">
+      <c r="C74" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D72" t="s">
-        <v>196</v>
-      </c>
-      <c r="E72" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="5" t="s">
-        <v>192</v>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>233</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D75" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="13" t="s">
-        <v>189</v>
+      <c r="A76" s="24"/>
+      <c r="B76" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D77" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
+      <c r="B78" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D78" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="24"/>
+      <c r="B79" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D79" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="24"/>
+      <c r="B80" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D80" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="23"/>
+      <c r="B81" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="B82" s="4"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="9"/>
-    </row>
-    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="B93" s="9"/>
+    </row>
+    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C93" s="22"/>
-    </row>
-    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>227</v>
+    <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="C96" s="22"/>
     </row>
     <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
-        <v>228</v>
+      <c r="A97" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C97" s="22"/>
     </row>
@@ -2736,83 +2776,99 @@
       <c r="C98" s="22"/>
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
+      <c r="A99" s="11" t="s">
+        <v>220</v>
+      </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
-        <v>39</v>
+      <c r="A100" s="11" t="s">
+        <v>221</v>
       </c>
       <c r="C100" s="22"/>
     </row>
     <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="A101" s="10"/>
       <c r="C101" s="22"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="A102" s="10"/>
       <c r="C102" s="22"/>
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
+      <c r="A105" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+      <c r="A106" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107" s="22"/>
+    </row>
+    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="10"/>
+      <c r="C108" s="22"/>
+    </row>
+    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="10"/>
+      <c r="C109" s="22"/>
+    </row>
+    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C107" s="22"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B108" s="9"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
+      <c r="B111" s="9"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A75:A80"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="A31:A37"/>
     <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A2:A28"/>
-    <mergeCell ref="A57:A65"/>
-    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A2:A30"/>
   </mergeCells>
-  <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  <dataValidations disablePrompts="1" count="11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B29" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
@@ -2822,27 +2878,31 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E36 E41" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$96:$A$97</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E38 E43" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>$A$99:$A$100</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E42:E43" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E39:E41 E44:E45" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$107:$A$108</formula1>
+      <formula1>$A$110:$A$111</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E48:E49" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E50:E51" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
       <formula2>4800</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E44" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E46" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A96:A97 E36 E41" numberStoredAsText="1"/>
+    <ignoredError sqref="A99:A100 E38 E43" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of readm and push to Github fof latest Orahub Changes (#113)
Update per latest terminology and ERs per feb 20th 2025
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5515ACC2-1EE6-4AB4-86BC-A25A734C0AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C92B609-4F14-45CC-BBA9-A40D42493029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7050" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="235">
   <si>
     <t>Yes</t>
   </si>
@@ -219,9 +218,6 @@
     <t>oci-network-ports-ons/port</t>
   </si>
   <si>
-    <t>oci-network-ports-wlsservers/port</t>
-  </si>
-  <si>
     <t>oci-wls-os_version/opt</t>
   </si>
   <si>
@@ -598,24 +594,6 @@
     <t>OPTIONAL Advanced  Configuration</t>
   </si>
   <si>
-    <t>Internal virtual host-LBR Port  (e.g. for internal accesses like OWSM)                   (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-Frontend Name                                      (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-LBR Port                                                    (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Virtual host for WebLogic Admin Console-OHS HTTP port                                        (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Internal virtual host-OHS HTTP port (e.g. for internal accesses like OWSM)        (leave blank if not used)</t>
-  </si>
-  <si>
-    <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)      (leave blank if not used)</t>
-  </si>
-  <si>
     <t>prem-ohs-listen_addresses/opt</t>
   </si>
   <si>
@@ -720,6 +698,45 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>WLS administration ports</t>
+  </si>
+  <si>
+    <t>WLS channels listen ports</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsadmin/port</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsservers/opt</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlschannels/opt</t>
+  </si>
+  <si>
+    <t>prem-wls-vipaddress/opt</t>
+  </si>
+  <si>
+    <t>If the Admin Server listens in a Virtual IP address, provide the virtual FQDN hostname value (e.g. asvip.example.com)    (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-OHS HTTP port                                                                                                                                 (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-Frontend Name                                                                                                                               (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-OHS HTTP port (e.g. for internal accesses like OWSM)                                                                                              (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-LBR Port  (e.g. for internal accesses like OWSM)                                                                                                          (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Internal virtual host-Frontend Name (e.g. for internal accesses like OWSM)                                                                                            (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Virtual host for WebLogic Admin Console-LBR Port                                                                                                                                              (leave blank if not used)</t>
   </si>
 </sst>
 </file>
@@ -727,7 +744,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -856,10 +873,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -904,6 +921,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1199,16 +1219,16 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X110"/>
+  <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="121.42578125" customWidth="1"/>
+    <col min="2" max="2" width="128.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
     <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
@@ -1226,106 +1246,106 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-    </row>
-    <row r="2" spans="1:24" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="C4" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
         <v>72</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -1335,48 +1355,48 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1393,18 +1413,18 @@
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1421,18 +1441,18 @@
       <c r="X11" s="6"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1450,18 +1470,18 @@
       <c r="X12" s="6"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1479,12 +1499,12 @@
       <c r="X13" s="6"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
@@ -1508,12 +1528,12 @@
       <c r="X14" s="6"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -1537,12 +1557,12 @@
       <c r="X15" s="6"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1566,12 +1586,12 @@
       <c r="X16" s="6"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -1595,18 +1615,18 @@
       <c r="X17" s="6"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1624,18 +1644,18 @@
       <c r="X18" s="6"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D19" t="s">
         <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1653,18 +1673,18 @@
       <c r="X19" s="6"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1682,18 +1702,18 @@
       <c r="X20" s="6"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1711,15 +1731,15 @@
       <c r="X21" s="6"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1740,12 +1760,12 @@
       <c r="X22" s="6"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1769,12 +1789,12 @@
       <c r="X23" s="6"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
@@ -1798,12 +1818,12 @@
       <c r="X24" s="6"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
@@ -1827,15 +1847,15 @@
       <c r="X25" s="6"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1856,15 +1876,15 @@
       <c r="X26" s="6"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1885,15 +1905,15 @@
       <c r="X27" s="6"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>225</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1911,823 +1931,843 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
-        <v>28</v>
-      </c>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>175</v>
+        <v>223</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>216</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C32" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" t="s">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25"/>
+      <c r="B34" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" t="s">
         <v>81</v>
       </c>
-      <c r="E31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D33" t="s">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="25"/>
+      <c r="B36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D36" t="s">
         <v>82</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" t="s">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D35" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C38" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" t="s">
         <v>63</v>
       </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" t="s">
         <v>64</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38">
+      <c r="E40">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="5" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39">
+      <c r="E41">
         <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E43" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="25"/>
+      <c r="B44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C45" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" t="s">
+        <v>192</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="25"/>
+      <c r="B46" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="B50" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+      <c r="B52" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
+      <c r="B53" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="24"/>
+      <c r="B54" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="24"/>
+      <c r="B55" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
+      <c r="B56" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
+      <c r="B57" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D57" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" t="s">
+        <v>205</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="24"/>
+      <c r="B60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D60" t="s">
+        <v>204</v>
+      </c>
+      <c r="E60" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+      <c r="B61" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" t="s">
-        <v>199</v>
-      </c>
-      <c r="E43">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C61" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" t="s">
+        <v>206</v>
+      </c>
+      <c r="E61" t="s">
         <v>200</v>
       </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" t="s">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="24"/>
+      <c r="B62" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" t="s">
-        <v>202</v>
-      </c>
-      <c r="E46">
-        <v>7777</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" t="s">
-        <v>113</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="C62" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+      <c r="B63" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49">
+      <c r="E63" t="s">
+        <v>155</v>
+      </c>
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="24"/>
+      <c r="B64" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="24"/>
+      <c r="B65" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D65" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="24"/>
+      <c r="B66" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" t="s">
-        <v>120</v>
-      </c>
-      <c r="E52" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" t="s">
-        <v>203</v>
-      </c>
-      <c r="E55">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" t="s">
-        <v>212</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" t="s">
-        <v>211</v>
-      </c>
-      <c r="E58" s="14">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D59" t="s">
-        <v>213</v>
-      </c>
-      <c r="E59" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" t="s">
-        <v>210</v>
-      </c>
-      <c r="E60">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D61" t="s">
-        <v>155</v>
-      </c>
-      <c r="E61" t="s">
-        <v>156</v>
-      </c>
-      <c r="F61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D62" t="s">
-        <v>182</v>
-      </c>
-      <c r="E62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" t="s">
-        <v>103</v>
-      </c>
-      <c r="E63" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D64" t="s">
-        <v>104</v>
-      </c>
-      <c r="E64" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D65" t="s">
-        <v>105</v>
-      </c>
-      <c r="E65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D66" t="s">
-        <v>216</v>
-      </c>
-      <c r="E66" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D67" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D68" t="s">
+        <v>209</v>
+      </c>
+      <c r="E68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="25"/>
+      <c r="B69" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D69" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="25"/>
+      <c r="B70" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="E67">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24"/>
-      <c r="B68" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D68" t="s">
-        <v>217</v>
-      </c>
-      <c r="E68" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="24"/>
-      <c r="B69" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D69" t="s">
-        <v>215</v>
-      </c>
-      <c r="E69">
+      <c r="C70" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D70" t="s">
+        <v>210</v>
+      </c>
+      <c r="E70" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="25"/>
+      <c r="B71" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D71" t="s">
+        <v>208</v>
+      </c>
+      <c r="E71">
         <v>1002</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="24"/>
-      <c r="B70" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D70" t="s">
-        <v>194</v>
-      </c>
-      <c r="E70" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="25"/>
+      <c r="B72" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D72" t="s">
+        <v>187</v>
+      </c>
+      <c r="E72" t="s">
+        <v>139</v>
+      </c>
+      <c r="F72" t="s">
         <v>140</v>
       </c>
-      <c r="F70" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="24"/>
-      <c r="B71" s="5" t="s">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="25"/>
+      <c r="B73" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D73" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" t="s">
         <v>159</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D71" t="s">
-        <v>195</v>
-      </c>
-      <c r="E71" t="s">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="25"/>
+      <c r="B74" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="24"/>
-      <c r="B72" s="5" t="s">
+      <c r="C74" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D72" t="s">
-        <v>196</v>
-      </c>
-      <c r="E72" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="5" t="s">
-        <v>192</v>
+    </row>
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>233</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D75" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="13" t="s">
-        <v>189</v>
+      <c r="A76" s="24"/>
+      <c r="B76" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="23"/>
+      <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D77" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
+      <c r="B78" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D78" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="24"/>
+      <c r="B79" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D79" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="24"/>
+      <c r="B80" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D80" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D78" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="23"/>
+      <c r="B81" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="B82" s="4"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B90" s="9"/>
-    </row>
-    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="B93" s="9"/>
+    </row>
+    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C93" s="22"/>
-    </row>
-    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>227</v>
+    <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="C96" s="22"/>
     </row>
     <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
-        <v>228</v>
+      <c r="A97" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="C97" s="22"/>
     </row>
@@ -2736,83 +2776,99 @@
       <c r="C98" s="22"/>
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
+      <c r="A99" s="11" t="s">
+        <v>220</v>
+      </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
-        <v>39</v>
+      <c r="A100" s="11" t="s">
+        <v>221</v>
       </c>
       <c r="C100" s="22"/>
     </row>
     <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="A101" s="10"/>
       <c r="C101" s="22"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="A102" s="10"/>
       <c r="C102" s="22"/>
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
+      <c r="A105" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+      <c r="A106" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107" s="22"/>
+    </row>
+    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="10"/>
+      <c r="C108" s="22"/>
+    </row>
+    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="10"/>
+      <c r="C109" s="22"/>
+    </row>
+    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C107" s="22"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B108" s="9"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
+      <c r="B111" s="9"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="A47:A55"/>
-    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A75:A80"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="A31:A37"/>
     <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A2:A28"/>
-    <mergeCell ref="A57:A65"/>
-    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A59:A67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A2:A30"/>
   </mergeCells>
-  <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+  <dataValidations disablePrompts="1" count="11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B29" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
@@ -2822,27 +2878,31 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E36 E41" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$96:$A$97</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E38 E43" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>$A$99:$A$100</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E37:E39 E42:E43" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E39:E41 E44:E45" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$107:$A$108</formula1>
+      <formula1>$A$110:$A$111</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E48:E49" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E50:E51" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
       <formula2>4800</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E44" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E46" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A96:A97 E36 E41" numberStoredAsText="1"/>
+    <ignoredError sqref="A99:A100 E38 E43" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added PEM comment to spreadshhet
For the LBR cert/key files
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C92B609-4F14-45CC-BBA9-A40D42493029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F37A8BA-CADB-4CB2-9ADD-58F56C3C419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -380,12 +380,6 @@
     <t>OCI Load Balancer</t>
   </si>
   <si>
-    <t>Public certificate path</t>
-  </si>
-  <si>
-    <t>Certificate private key</t>
-  </si>
-  <si>
     <t>oci-lbr-public_certificate/path</t>
   </si>
   <si>
@@ -737,6 +731,12 @@
   </si>
   <si>
     <t>Virtual host for WebLogic Admin Console-LBR Port                                                                                                                                              (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Public certificate path (in PEM format)</t>
+  </si>
+  <si>
+    <t>Certificate private key (in PEM format)</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -873,7 +873,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -1221,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1246,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
@@ -1270,7 +1270,7 @@
         <v>83</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -1285,13 +1285,13 @@
         <v>65</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1300,13 +1300,13 @@
         <v>67</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1315,13 +1315,13 @@
         <v>87</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -1345,7 +1345,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -1357,31 +1357,31 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,13 +1390,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
         <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1418,13 +1418,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
         <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1446,13 +1446,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
         <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1475,13 +1475,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
         <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1504,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
@@ -1533,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -1562,7 +1562,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1591,7 +1591,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -1620,13 +1620,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1649,13 +1649,13 @@
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" t="s">
         <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1678,13 +1678,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1707,13 +1707,13 @@
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1736,7 +1736,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D22" t="s">
         <v>105</v>
@@ -1765,7 +1765,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1794,7 +1794,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
@@ -1823,7 +1823,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
@@ -1849,13 +1849,13 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1878,13 +1878,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1910,10 +1910,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1934,25 +1934,25 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" t="s">
         <v>222</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D30" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1963,13 +1963,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
         <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,13 +1978,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D32" t="s">
         <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1993,13 +1993,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D33" t="s">
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2008,13 +2008,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D34" t="s">
         <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
         <v>32</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
         <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2038,13 +2038,13 @@
         <v>33</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
         <v>82</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,13 +2053,13 @@
         <v>73</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" t="s">
         <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2070,13 +2070,13 @@
         <v>38</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
         <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,7 +2085,7 @@
         <v>45</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -2100,7 +2100,7 @@
         <v>46</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
@@ -2115,7 +2115,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
         <v>70</v>
@@ -2130,30 +2130,30 @@
         <v>68</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
         <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s">
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2162,10 +2162,10 @@
         <v>91</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2177,10 +2177,10 @@
         <v>92</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E45">
         <v>16</v>
@@ -2192,10 +2192,10 @@
         <v>93</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2207,25 +2207,25 @@
         <v>94</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E48">
         <v>7777</v>
@@ -2239,22 +2239,22 @@
         <v>111</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D49" t="s">
         <v>112</v>
       </c>
       <c r="E49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
         <v>113</v>
@@ -2266,10 +2266,10 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>114</v>
@@ -2281,82 +2281,82 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" t="s">
-        <v>118</v>
-      </c>
       <c r="E52" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D54" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" t="s">
-        <v>119</v>
-      </c>
       <c r="E54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D56" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" t="s">
-        <v>128</v>
-      </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E57">
         <v>443</v>
@@ -2370,7 +2370,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>58</v>
@@ -2384,28 +2384,28 @@
         <v>97</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" t="s">
-        <v>205</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" t="s">
         <v>202</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" t="s">
-        <v>204</v>
       </c>
       <c r="E60" s="14">
         <v>1001</v>
@@ -2414,28 +2414,28 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" t="s">
         <v>198</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" t="s">
-        <v>206</v>
-      </c>
-      <c r="E61" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" t="s">
         <v>201</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D62" t="s">
-        <v>203</v>
       </c>
       <c r="E62">
         <v>1002</v>
@@ -2444,31 +2444,31 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" t="s">
         <v>154</v>
-      </c>
-      <c r="E63" t="s">
-        <v>155</v>
-      </c>
-      <c r="F63" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" t="s">
         <v>179</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D64" t="s">
-        <v>181</v>
       </c>
       <c r="E64" t="s">
         <v>99</v>
@@ -2477,10 +2477,10 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
         <v>102</v>
@@ -2492,10 +2492,10 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D66" t="s">
         <v>103</v>
@@ -2507,45 +2507,45 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
         <v>104</v>
       </c>
       <c r="E67" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E68" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E69">
         <v>1001</v>
@@ -2554,28 +2554,28 @@
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25"/>
       <c r="B70" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E71">
         <v>1002</v>
@@ -2587,132 +2587,132 @@
         <v>98</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D78" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2777,13 +2777,13 @@
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C100" s="22"/>
     </row>

</xml_diff>

<commit_message>
Added PEM comment to spreadshhet (#135)
For the LBR cert/key files
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C92B609-4F14-45CC-BBA9-A40D42493029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F37A8BA-CADB-4CB2-9ADD-58F56C3C419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -380,12 +380,6 @@
     <t>OCI Load Balancer</t>
   </si>
   <si>
-    <t>Public certificate path</t>
-  </si>
-  <si>
-    <t>Certificate private key</t>
-  </si>
-  <si>
     <t>oci-lbr-public_certificate/path</t>
   </si>
   <si>
@@ -737,6 +731,12 @@
   </si>
   <si>
     <t>Virtual host for WebLogic Admin Console-LBR Port                                                                                                                                              (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>Public certificate path (in PEM format)</t>
+  </si>
+  <si>
+    <t>Certificate private key (in PEM format)</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -873,7 +873,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -1221,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1246,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
@@ -1270,7 +1270,7 @@
         <v>83</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D2" t="s">
         <v>84</v>
@@ -1285,13 +1285,13 @@
         <v>65</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1300,13 +1300,13 @@
         <v>67</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D4" t="s">
         <v>88</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1315,13 +1315,13 @@
         <v>87</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
         <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
         <v>72</v>
@@ -1345,7 +1345,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -1357,31 +1357,31 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,13 +1390,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
         <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1418,13 +1418,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
         <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1446,13 +1446,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
         <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1475,13 +1475,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
         <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1504,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
@@ -1533,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
@@ -1562,7 +1562,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -1591,7 +1591,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -1620,13 +1620,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1649,13 +1649,13 @@
         <v>12</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" t="s">
         <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1678,13 +1678,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1707,13 +1707,13 @@
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1736,7 +1736,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D22" t="s">
         <v>105</v>
@@ -1765,7 +1765,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D23" t="s">
         <v>59</v>
@@ -1794,7 +1794,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
@@ -1823,7 +1823,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D25" t="s">
         <v>61</v>
@@ -1849,13 +1849,13 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1878,13 +1878,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1910,10 +1910,10 @@
         <v>23</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1934,25 +1934,25 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" t="s">
         <v>222</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="D30" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1963,13 +1963,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
         <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1978,13 +1978,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D32" t="s">
         <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1993,13 +1993,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D33" t="s">
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2008,13 +2008,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D34" t="s">
         <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
         <v>32</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
         <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2038,13 +2038,13 @@
         <v>33</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" t="s">
         <v>82</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,13 +2053,13 @@
         <v>73</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D37" t="s">
         <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2070,13 +2070,13 @@
         <v>38</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
         <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,7 +2085,7 @@
         <v>45</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
         <v>63</v>
@@ -2100,7 +2100,7 @@
         <v>46</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
@@ -2115,7 +2115,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D41" t="s">
         <v>70</v>
@@ -2130,30 +2130,30 @@
         <v>68</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
         <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D43" t="s">
         <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2162,10 +2162,10 @@
         <v>91</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2177,10 +2177,10 @@
         <v>92</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E45">
         <v>16</v>
@@ -2192,10 +2192,10 @@
         <v>93</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2207,25 +2207,25 @@
         <v>94</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E48">
         <v>7777</v>
@@ -2239,22 +2239,22 @@
         <v>111</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D49" t="s">
         <v>112</v>
       </c>
       <c r="E49" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D50" t="s">
         <v>113</v>
@@ -2266,10 +2266,10 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D51" t="s">
         <v>114</v>
@@ -2281,82 +2281,82 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D52" t="s">
         <v>116</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" t="s">
-        <v>118</v>
-      </c>
       <c r="E52" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D54" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" t="s">
-        <v>119</v>
-      </c>
       <c r="E54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D56" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" t="s">
-        <v>128</v>
-      </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E57">
         <v>443</v>
@@ -2370,7 +2370,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D58" s="14" t="s">
         <v>58</v>
@@ -2384,28 +2384,28 @@
         <v>97</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" t="s">
-        <v>205</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" t="s">
         <v>202</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" t="s">
-        <v>204</v>
       </c>
       <c r="E60" s="14">
         <v>1001</v>
@@ -2414,28 +2414,28 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" t="s">
         <v>198</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" t="s">
-        <v>206</v>
-      </c>
-      <c r="E61" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" t="s">
         <v>201</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D62" t="s">
-        <v>203</v>
       </c>
       <c r="E62">
         <v>1002</v>
@@ -2444,31 +2444,31 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D63" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" t="s">
         <v>154</v>
-      </c>
-      <c r="E63" t="s">
-        <v>155</v>
-      </c>
-      <c r="F63" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" t="s">
         <v>179</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D64" t="s">
-        <v>181</v>
       </c>
       <c r="E64" t="s">
         <v>99</v>
@@ -2477,10 +2477,10 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D65" t="s">
         <v>102</v>
@@ -2492,10 +2492,10 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D66" t="s">
         <v>103</v>
@@ -2507,45 +2507,45 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
         <v>104</v>
       </c>
       <c r="E67" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D68" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E68" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E69">
         <v>1001</v>
@@ -2554,28 +2554,28 @@
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25"/>
       <c r="B70" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E71">
         <v>1002</v>
@@ -2587,132 +2587,132 @@
         <v>98</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D72" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D73" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D78" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -2777,13 +2777,13 @@
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C100" s="22"/>
     </row>

</xml_diff>

<commit_message>
added clarification to the subnet rows
added "(if it already exists, it will be reused)"
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F37A8BA-CADB-4CB2-9ADD-58F56C3C419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF7205C-8FB3-44C1-B610-CB78A2049745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,18 +36,6 @@
     <t>10.100.100.0/24</t>
   </si>
   <si>
-    <t>Webtier Subnet Name</t>
-  </si>
-  <si>
-    <t>Dbtier Subnet Name</t>
-  </si>
-  <si>
-    <t>Fsstier Subnet Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midtier Subnet Name </t>
-  </si>
-  <si>
     <t>Is the webtier private?</t>
   </si>
   <si>
@@ -737,6 +725,18 @@
   </si>
   <si>
     <t>Certificate private key (in PEM format)</t>
+  </si>
+  <si>
+    <t>Webtier Subnet Name           (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Midtier Subnet Name             (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Dbtier Subnet Name                (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Fsstier Subnet Name               (if it already exists, it will be reused)</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,20 +1240,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
@@ -1264,76 +1264,76 @@
     </row>
     <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1342,13 +1342,13 @@
     <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -1357,46 +1357,46 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
-        <v>3</v>
+        <v>231</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1415,16 +1415,16 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1443,16 +1443,16 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1472,16 +1472,16 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
-        <v>5</v>
+        <v>234</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1501,13 +1501,13 @@
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1530,13 +1530,13 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -1559,13 +1559,13 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -1588,13 +1588,13 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1617,16 +1617,16 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1646,16 +1646,16 @@
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1675,16 +1675,16 @@
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1704,16 +1704,16 @@
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1733,13 +1733,13 @@
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1762,13 +1762,13 @@
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E23" s="7">
         <v>22</v>
@@ -1791,13 +1791,13 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E24" s="8">
         <v>1521</v>
@@ -1820,13 +1820,13 @@
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E25">
         <v>6200</v>
@@ -1849,13 +1849,13 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1878,13 +1878,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1907,13 +1907,13 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D28" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1934,161 +1934,161 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D29" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D30" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2097,13 +2097,13 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E40">
         <v>16</v>
@@ -2112,13 +2112,13 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2127,45 +2127,45 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2174,13 +2174,13 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E45">
         <v>16</v>
@@ -2189,13 +2189,13 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2204,28 +2204,28 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D48" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E48">
         <v>7777</v>
@@ -2233,31 +2233,31 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E49" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E50">
         <v>10</v>
@@ -2266,13 +2266,13 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E51">
         <v>100</v>
@@ -2281,82 +2281,82 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D52" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D56" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E57">
         <v>443</v>
@@ -2364,16 +2364,16 @@
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>2</v>
@@ -2381,31 +2381,31 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D60" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E60" s="14">
         <v>1001</v>
@@ -2414,28 +2414,28 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D61" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E62">
         <v>1002</v>
@@ -2444,108 +2444,108 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D63" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E63" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E64" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D65" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E65" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E67" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E69">
         <v>1001</v>
@@ -2554,28 +2554,28 @@
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25"/>
       <c r="B70" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E70" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D71" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E71">
         <v>1002</v>
@@ -2584,140 +2584,140 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D72" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E72" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D73" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E73" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D74" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E74" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D77" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="20"/>
@@ -2726,17 +2726,17 @@
     </row>
     <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2761,13 +2761,13 @@
     </row>
     <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C96" s="22"/>
     </row>
     <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C97" s="22"/>
     </row>
@@ -2777,13 +2777,13 @@
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C100" s="22"/>
     </row>
@@ -2797,31 +2797,31 @@
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C107" s="22"/>
     </row>
@@ -2835,13 +2835,13 @@
     </row>
     <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C110" s="22"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B111" s="9"/>
     </row>
@@ -2865,7 +2865,7 @@
     <mergeCell ref="A68:A74"/>
     <mergeCell ref="A2:A30"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="11">
+  <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
added clarification to the subnet rows (#137)
added "(if it already exists, it will be reused)"
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F37A8BA-CADB-4CB2-9ADD-58F56C3C419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF7205C-8FB3-44C1-B610-CB78A2049745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,18 +36,6 @@
     <t>10.100.100.0/24</t>
   </si>
   <si>
-    <t>Webtier Subnet Name</t>
-  </si>
-  <si>
-    <t>Dbtier Subnet Name</t>
-  </si>
-  <si>
-    <t>Fsstier Subnet Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midtier Subnet Name </t>
-  </si>
-  <si>
     <t>Is the webtier private?</t>
   </si>
   <si>
@@ -737,6 +725,18 @@
   </si>
   <si>
     <t>Certificate private key (in PEM format)</t>
+  </si>
+  <si>
+    <t>Webtier Subnet Name           (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Midtier Subnet Name             (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Dbtier Subnet Name                (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Fsstier Subnet Name               (if it already exists, it will be reused)</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,20 +1240,20 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
@@ -1264,76 +1264,76 @@
     </row>
     <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
@@ -1342,13 +1342,13 @@
     <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -1357,46 +1357,46 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
-        <v>3</v>
+        <v>231</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1415,16 +1415,16 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1443,16 +1443,16 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
-        <v>4</v>
+        <v>233</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1472,16 +1472,16 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
-        <v>5</v>
+        <v>234</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1501,13 +1501,13 @@
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
@@ -1530,13 +1530,13 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
@@ -1559,13 +1559,13 @@
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
@@ -1588,13 +1588,13 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
@@ -1617,16 +1617,16 @@
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1646,16 +1646,16 @@
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1675,16 +1675,16 @@
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1704,16 +1704,16 @@
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1733,13 +1733,13 @@
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1762,13 +1762,13 @@
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E23" s="7">
         <v>22</v>
@@ -1791,13 +1791,13 @@
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E24" s="8">
         <v>1521</v>
@@ -1820,13 +1820,13 @@
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E25">
         <v>6200</v>
@@ -1849,13 +1849,13 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E26">
         <v>5556</v>
@@ -1878,13 +1878,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1907,13 +1907,13 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D28" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E28">
         <v>7010</v>
@@ -1934,161 +1934,161 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D29" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D30" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -2097,13 +2097,13 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E40">
         <v>16</v>
@@ -2112,13 +2112,13 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -2127,45 +2127,45 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E43" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -2174,13 +2174,13 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E45">
         <v>16</v>
@@ -2189,13 +2189,13 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -2204,28 +2204,28 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D48" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E48">
         <v>7777</v>
@@ -2233,31 +2233,31 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D49" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E49" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E50">
         <v>10</v>
@@ -2266,13 +2266,13 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D51" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E51">
         <v>100</v>
@@ -2281,82 +2281,82 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D52" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E54" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D56" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E56" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D57" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E57">
         <v>443</v>
@@ -2364,16 +2364,16 @@
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>2</v>
@@ -2381,31 +2381,31 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
       <c r="B60" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D60" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E60" s="14">
         <v>1001</v>
@@ -2414,28 +2414,28 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D61" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E62">
         <v>1002</v>
@@ -2444,108 +2444,108 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D63" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E63" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F63" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E64" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D65" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E65" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E67" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E69">
         <v>1001</v>
@@ -2554,28 +2554,28 @@
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="25"/>
       <c r="B70" s="5" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E70" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D71" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E71">
         <v>1002</v>
@@ -2584,140 +2584,140 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D72" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E72" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D73" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E73" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D74" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E74" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D77" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="20"/>
@@ -2726,17 +2726,17 @@
     </row>
     <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2761,13 +2761,13 @@
     </row>
     <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C96" s="22"/>
     </row>
     <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C97" s="22"/>
     </row>
@@ -2777,13 +2777,13 @@
     </row>
     <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C99" s="22"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C100" s="22"/>
     </row>
@@ -2797,31 +2797,31 @@
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C107" s="22"/>
     </row>
@@ -2835,13 +2835,13 @@
     </row>
     <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C110" s="22"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B111" s="9"/>
     </row>
@@ -2865,7 +2865,7 @@
     <mergeCell ref="A68:A74"/>
     <mergeCell ref="A2:A30"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="11">
+  <dataValidations count="11">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
Last updates from orahub
This commit is to include the last merges not yet pushed to GitHub:
- Resolve "Support for scenarios when the JDK is not under the products folder"
- Resolve "Use higher paramiko version to support OPENSSH Key formats"
- 114 112 106 91 (among other minor fixes, the change to use SOA image)
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF7205C-8FB3-44C1-B610-CB78A2049745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ADC43D-C795-4FD8-9927-1ECA1A0431B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="243">
   <si>
     <t>Yes</t>
   </si>
@@ -407,13 +407,7 @@
     <t>oci-network-ports-node_manager/port</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence/port</t>
-  </si>
-  <si>
     <t>NodeManager port</t>
-  </si>
-  <si>
-    <t>Coherence port</t>
   </si>
   <si>
     <t>10.1.1.0/24</t>
@@ -649,18 +643,6 @@
     <t>prem-ohs-group_name/opt</t>
   </si>
   <si>
-    <t>OSH owner OS user name</t>
-  </si>
-  <si>
-    <t>OSH owner OS user ID</t>
-  </si>
-  <si>
-    <t>OSH owner OS group ID</t>
-  </si>
-  <si>
-    <t>OSH owner OS group name</t>
-  </si>
-  <si>
     <t>/u02</t>
   </si>
   <si>
@@ -688,9 +670,6 @@
     <t>WLS channels listen ports</t>
   </si>
   <si>
-    <t>oci-network-ports-wlsadmin/port</t>
-  </si>
-  <si>
     <t>oci-network-ports-wlsservers/opt</t>
   </si>
   <si>
@@ -737,6 +716,51 @@
   </si>
   <si>
     <t>Fsstier Subnet Name               (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Coherence cluster ports (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_cluster/port</t>
+  </si>
+  <si>
+    <t>Coherence unicast ports (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_unicast/port</t>
+  </si>
+  <si>
+    <t>Is this a SOA Domain? (e.g. it has any product of the SOA Suite like SOA, BPM, OSB or MFT)</t>
+  </si>
+  <si>
+    <t>prem-wls-is_soa/yesno</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsadmin/opt</t>
+  </si>
+  <si>
+    <t>OHS owner OS user name</t>
+  </si>
+  <si>
+    <t>OHS owner OS user ID</t>
+  </si>
+  <si>
+    <t>OHS owner OS group name</t>
+  </si>
+  <si>
+    <t>OHS owner OS group ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the OHS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products directory path) </t>
+  </si>
+  <si>
+    <t>prem-ohs-jdk_path/opt</t>
+  </si>
+  <si>
+    <t>prem-wls-jdk_path/opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the WLS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products mountpoint) </t>
   </si>
 </sst>
 </file>
@@ -744,7 +768,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -873,10 +897,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -922,17 +946,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1219,10 +1240,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X113"/>
+  <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,21 +1267,21 @@
         <v>14</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -1270,7 +1291,7 @@
         <v>79</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -1285,13 +1306,13 @@
         <v>61</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1300,13 +1321,13 @@
         <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1315,13 +1336,13 @@
         <v>83</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
         <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1330,7 +1351,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
@@ -1345,7 +1366,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1357,46 +1378,46 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
         <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1415,16 +1436,16 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
         <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1443,16 +1464,16 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1472,16 +1493,16 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
         <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1504,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1533,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1562,7 +1583,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
         <v>48</v>
@@ -1591,7 +1612,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1620,13 +1641,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1649,13 +1670,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1678,13 +1699,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
         <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1707,13 +1728,13 @@
         <v>10</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1736,7 +1757,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D22" t="s">
         <v>101</v>
@@ -1765,7 +1786,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D23" t="s">
         <v>55</v>
@@ -1794,7 +1815,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
@@ -1823,7 +1844,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
@@ -1849,10 +1870,10 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
         <v>124</v>
@@ -1878,13 +1899,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1907,571 +1928,597 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E28">
-        <v>7010</v>
+        <v>8876</v>
       </c>
       <c r="F28">
-        <v>8001</v>
+        <v>8877</v>
       </c>
       <c r="G28">
-        <v>8011</v>
+        <v>8878</v>
       </c>
       <c r="H28">
-        <v>8021</v>
+        <v>8879</v>
       </c>
       <c r="I28">
-        <v>9001</v>
-      </c>
+        <v>8880</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>210</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>220</v>
+        <v>212</v>
+      </c>
+      <c r="E29">
+        <v>7010</v>
+      </c>
+      <c r="F29">
+        <v>8001</v>
+      </c>
+      <c r="G29">
+        <v>8011</v>
+      </c>
+      <c r="H29">
+        <v>8021</v>
+      </c>
+      <c r="I29">
+        <v>9001</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C30" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="C31" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="E31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" t="s">
         <v>70</v>
       </c>
-      <c r="E37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="E38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C39" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" t="s">
         <v>58</v>
       </c>
-      <c r="E38" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D39" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" t="s">
         <v>71</v>
       </c>
-      <c r="E42" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="E43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" t="s">
         <v>91</v>
       </c>
-      <c r="E43" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D44" t="s">
-        <v>185</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
+      <c r="E44" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E45">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D47" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" t="s">
-        <v>166</v>
+        <v>185</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="25"/>
+      <c r="B49" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" t="s">
-        <v>189</v>
-      </c>
-      <c r="E48">
+      <c r="C49" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49">
         <v>7777</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C50" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
         <v>108</v>
       </c>
-      <c r="E49" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
+      <c r="E50" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>167</v>
+        <v>117</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" t="s">
-        <v>156</v>
+        <v>110</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
-        <v>230</v>
+        <v>123</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D54" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
-      </c>
-      <c r="E56" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+      <c r="B58" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" t="s">
-        <v>190</v>
-      </c>
-      <c r="E57">
+      <c r="C58" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58">
         <v>443</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D58" s="14" t="s">
+      <c r="C59" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E59" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" t="s">
-        <v>199</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" s="14">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
-      </c>
-      <c r="E61" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="E61" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D62" t="s">
-        <v>197</v>
-      </c>
-      <c r="E62">
-        <v>1002</v>
+        <v>198</v>
+      </c>
+      <c r="E62" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D63" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" t="s">
-        <v>150</v>
+        <v>195</v>
+      </c>
+      <c r="E63">
+        <v>1002</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D64" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="E64" t="s">
-        <v>95</v>
+        <v>147</v>
+      </c>
+      <c r="F64" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2480,315 +2527,349 @@
         <v>171</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="E65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E66" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68" t="s">
         <v>100</v>
       </c>
-      <c r="E67" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>203</v>
       </c>
-      <c r="E68" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
       <c r="B69" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>167</v>
+        <v>242</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="D69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70" t="s">
         <v>201</v>
       </c>
-      <c r="E69">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
-      <c r="B70" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" t="s">
-        <v>204</v>
-      </c>
       <c r="E70" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E71">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>94</v>
+        <v>237</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="E72" t="s">
-        <v>133</v>
-      </c>
-      <c r="F72" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D73" t="s">
-        <v>182</v>
-      </c>
-      <c r="E73" t="s">
-        <v>153</v>
+        <v>200</v>
+      </c>
+      <c r="E73">
+        <v>1002</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E74" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75" t="s">
         <v>180</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D75" t="s">
-        <v>164</v>
+      <c r="E75" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>210</v>
+        <v>152</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>181</v>
+      </c>
+      <c r="E76" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="5" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="B78" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D78" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D79" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D80" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="5" t="s">
-        <v>222</v>
+      <c r="A81" s="24"/>
+      <c r="B81" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D81" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="24"/>
+      <c r="B82" s="5" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+      <c r="C82" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="24"/>
+      <c r="B83" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="24"/>
+      <c r="B84" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="24"/>
+      <c r="B85" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B86" s="4"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="9"/>
-    </row>
-    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+      <c r="B97" s="9"/>
+    </row>
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C94" s="22"/>
-    </row>
-    <row r="95" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
-      <c r="C95" s="22"/>
-    </row>
-    <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C96" s="22"/>
-    </row>
-    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C97" s="22"/>
-    </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-      <c r="C98" s="22"/>
-    </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C99" s="22"/>
-    </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C100" s="22"/>
-    </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10"/>
       <c r="C101" s="22"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2796,102 +2877,122 @@
       <c r="C102" s="22"/>
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
-        <v>35</v>
+      <c r="A103" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
-        <v>36</v>
+      <c r="A104" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="A105" s="10"/>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="A106" s="10"/>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C107" s="22"/>
     </row>
     <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+      <c r="A108" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="C108" s="22"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
+      <c r="A109" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="C109" s="22"/>
     </row>
     <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C111" s="22"/>
+    </row>
+    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="10"/>
+      <c r="C112" s="22"/>
+    </row>
+    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="10"/>
+      <c r="C113" s="22"/>
+    </row>
+    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C110" s="22"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
+      <c r="C114" s="22"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B111" s="9"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="9"/>
-      <c r="B112" s="9"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
+      <c r="B115" s="9"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A75:A80"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="A31:A37"/>
     <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A78:A85"/>
+    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A2:A31"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="A32:A38"/>
   </mergeCells>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B29:B31" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B32" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22 E6:E7 E15:E17" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22 E6:E7 E15:E17 E85" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E38 E43" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$99:$A$100</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E39 E44" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>$A$103:$A$104</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E39:E41 E44:E45" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E40:E42 E45:E46" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$110:$A$111</formula1>
+      <formula1>$A$114:$A$115</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E50:E51" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E51:E52" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
       <formula2>4800</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E46" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E47" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2902,7 +3003,7 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A99:A100 E38 E43" numberStoredAsText="1"/>
+    <ignoredError sqref="A103:A104 E39 E44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last updates from orahub (#139)
This commit is to include the last merges not yet pushed to GitHub:
- Resolve "Support for scenarios when the JDK is not under the products folder"
- Resolve "Use higher paramiko version to support OPENSSH Key formats"
- 114 112 106 91 (among other minor fixes, the change to use SOA image)
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\OraHubProjects\fmw-maa\wls-hydr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF7205C-8FB3-44C1-B610-CB78A2049745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ADC43D-C795-4FD8-9927-1ECA1A0431B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="243">
   <si>
     <t>Yes</t>
   </si>
@@ -407,13 +407,7 @@
     <t>oci-network-ports-node_manager/port</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence/port</t>
-  </si>
-  <si>
     <t>NodeManager port</t>
-  </si>
-  <si>
-    <t>Coherence port</t>
   </si>
   <si>
     <t>10.1.1.0/24</t>
@@ -649,18 +643,6 @@
     <t>prem-ohs-group_name/opt</t>
   </si>
   <si>
-    <t>OSH owner OS user name</t>
-  </si>
-  <si>
-    <t>OSH owner OS user ID</t>
-  </si>
-  <si>
-    <t>OSH owner OS group ID</t>
-  </si>
-  <si>
-    <t>OSH owner OS group name</t>
-  </si>
-  <si>
     <t>/u02</t>
   </si>
   <si>
@@ -688,9 +670,6 @@
     <t>WLS channels listen ports</t>
   </si>
   <si>
-    <t>oci-network-ports-wlsadmin/port</t>
-  </si>
-  <si>
     <t>oci-network-ports-wlsservers/opt</t>
   </si>
   <si>
@@ -737,6 +716,51 @@
   </si>
   <si>
     <t>Fsstier Subnet Name               (if it already exists, it will be reused)</t>
+  </si>
+  <si>
+    <t>Coherence cluster ports (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_cluster/port</t>
+  </si>
+  <si>
+    <t>Coherence unicast ports (leave blank if not used)</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_unicast/port</t>
+  </si>
+  <si>
+    <t>Is this a SOA Domain? (e.g. it has any product of the SOA Suite like SOA, BPM, OSB or MFT)</t>
+  </si>
+  <si>
+    <t>prem-wls-is_soa/yesno</t>
+  </si>
+  <si>
+    <t>oci-network-ports-wlsadmin/opt</t>
+  </si>
+  <si>
+    <t>OHS owner OS user name</t>
+  </si>
+  <si>
+    <t>OHS owner OS user ID</t>
+  </si>
+  <si>
+    <t>OHS owner OS group name</t>
+  </si>
+  <si>
+    <t>OHS owner OS group ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the OHS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products directory path) </t>
+  </si>
+  <si>
+    <t>prem-ohs-jdk_path/opt</t>
+  </si>
+  <si>
+    <t>prem-wls-jdk_path/opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the WLS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products mountpoint) </t>
   </si>
 </sst>
 </file>
@@ -744,7 +768,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -873,10 +897,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -922,17 +946,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1219,10 +1240,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X113"/>
+  <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,21 +1267,21 @@
         <v>14</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -1270,7 +1291,7 @@
         <v>79</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -1285,13 +1306,13 @@
         <v>61</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1300,13 +1321,13 @@
         <v>63</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1315,13 +1336,13 @@
         <v>83</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
         <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1330,7 +1351,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
         <v>68</v>
@@ -1345,7 +1366,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1357,46 +1378,46 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
         <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1415,16 +1436,16 @@
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
         <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1443,16 +1464,16 @@
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>104</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1472,16 +1493,16 @@
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
         <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1504,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1533,7 +1554,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1562,7 +1583,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
         <v>48</v>
@@ -1591,7 +1612,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1620,13 +1641,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1649,13 +1670,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
         <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1678,13 +1699,13 @@
         <v>9</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
         <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1707,13 +1728,13 @@
         <v>10</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1736,7 +1757,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D22" t="s">
         <v>101</v>
@@ -1765,7 +1786,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D23" t="s">
         <v>55</v>
@@ -1794,7 +1815,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D24" t="s">
         <v>56</v>
@@ -1823,7 +1844,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
         <v>57</v>
@@ -1849,10 +1870,10 @@
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
         <v>124</v>
@@ -1878,13 +1899,13 @@
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
-        <v>127</v>
+        <v>228</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1907,571 +1928,597 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E28">
-        <v>7010</v>
+        <v>8876</v>
       </c>
       <c r="F28">
-        <v>8001</v>
+        <v>8877</v>
       </c>
       <c r="G28">
-        <v>8011</v>
+        <v>8878</v>
       </c>
       <c r="H28">
-        <v>8021</v>
+        <v>8879</v>
       </c>
       <c r="I28">
-        <v>9001</v>
-      </c>
+        <v>8880</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>210</v>
+        <v>19</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>220</v>
+        <v>212</v>
+      </c>
+      <c r="E29">
+        <v>7010</v>
+      </c>
+      <c r="F29">
+        <v>8001</v>
+      </c>
+      <c r="G29">
+        <v>8011</v>
+      </c>
+      <c r="H29">
+        <v>8021</v>
+      </c>
+      <c r="I29">
+        <v>9001</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C30" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="D30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="C31" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="E31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C38" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" t="s">
         <v>70</v>
       </c>
-      <c r="E37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="E38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C39" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" t="s">
         <v>58</v>
       </c>
-      <c r="E38" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D39" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" t="s">
         <v>71</v>
       </c>
-      <c r="E42" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="E43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" t="s">
         <v>91</v>
       </c>
-      <c r="E43" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D44" t="s">
-        <v>185</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
+      <c r="E44" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E45">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D46" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D47" t="s">
-        <v>188</v>
-      </c>
-      <c r="E47" t="s">
-        <v>166</v>
+        <v>185</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="25"/>
+      <c r="B49" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" t="s">
-        <v>189</v>
-      </c>
-      <c r="E48">
+      <c r="C49" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49">
         <v>7777</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C50" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
         <v>108</v>
       </c>
-      <c r="E49" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
+      <c r="E50" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>167</v>
+        <v>117</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" t="s">
-        <v>156</v>
+        <v>110</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
-        <v>230</v>
+        <v>123</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D54" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
-      </c>
-      <c r="E56" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+      <c r="B58" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" t="s">
-        <v>190</v>
-      </c>
-      <c r="E57">
+      <c r="C58" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" t="s">
+        <v>188</v>
+      </c>
+      <c r="E58">
         <v>443</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D58" s="14" t="s">
+      <c r="C59" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E59" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B60" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" t="s">
-        <v>199</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" s="14">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
-      </c>
-      <c r="E61" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="E61" s="14">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D62" t="s">
-        <v>197</v>
-      </c>
-      <c r="E62">
-        <v>1002</v>
+        <v>198</v>
+      </c>
+      <c r="E62" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D63" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" t="s">
-        <v>149</v>
-      </c>
-      <c r="F63" t="s">
-        <v>150</v>
+        <v>195</v>
+      </c>
+      <c r="E63">
+        <v>1002</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D64" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="E64" t="s">
-        <v>95</v>
+        <v>147</v>
+      </c>
+      <c r="F64" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2480,315 +2527,349 @@
         <v>171</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="E65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E66" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68" t="s">
         <v>100</v>
       </c>
-      <c r="E67" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>203</v>
       </c>
-      <c r="E68" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
       <c r="B69" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>167</v>
+        <v>242</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>204</v>
       </c>
       <c r="D69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70" t="s">
         <v>201</v>
       </c>
-      <c r="E69">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
-      <c r="B70" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" t="s">
-        <v>204</v>
-      </c>
       <c r="E70" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E71">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>94</v>
+        <v>237</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="E72" t="s">
-        <v>133</v>
-      </c>
-      <c r="F72" t="s">
-        <v>134</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>152</v>
+        <v>238</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D73" t="s">
-        <v>182</v>
-      </c>
-      <c r="E73" t="s">
-        <v>153</v>
+        <v>200</v>
+      </c>
+      <c r="E73">
+        <v>1002</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E74" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="F74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75" t="s">
         <v>180</v>
       </c>
-      <c r="B75" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D75" t="s">
-        <v>164</v>
+      <c r="E75" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>210</v>
+        <v>152</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D76" t="s">
-        <v>165</v>
+        <v>181</v>
+      </c>
+      <c r="E76" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="5" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
+        <v>178</v>
+      </c>
       <c r="B78" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D78" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D79" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D80" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="5" t="s">
-        <v>222</v>
+      <c r="A81" s="24"/>
+      <c r="B81" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D81" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="24"/>
+      <c r="B82" s="5" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
+      <c r="C82" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="24"/>
+      <c r="B83" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="24"/>
+      <c r="B84" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="24"/>
+      <c r="B85" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" t="s">
+        <v>233</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B86" s="4"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="9"/>
-    </row>
-    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+      <c r="B97" s="9"/>
+    </row>
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C94" s="22"/>
-    </row>
-    <row r="95" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
-      <c r="C95" s="22"/>
-    </row>
-    <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
+      <c r="C98" s="22"/>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="C99" s="22"/>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C96" s="22"/>
-    </row>
-    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
+      <c r="C100" s="22"/>
+    </row>
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C97" s="22"/>
-    </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-      <c r="C98" s="22"/>
-    </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C99" s="22"/>
-    </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C100" s="22"/>
-    </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10"/>
       <c r="C101" s="22"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2796,102 +2877,122 @@
       <c r="C102" s="22"/>
     </row>
     <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
-        <v>35</v>
+      <c r="A103" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="C103" s="22"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
-        <v>36</v>
+      <c r="A104" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="C104" s="22"/>
     </row>
     <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="A105" s="10"/>
       <c r="C105" s="22"/>
     </row>
     <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="A106" s="10"/>
       <c r="C106" s="22"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C107" s="22"/>
     </row>
     <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="10"/>
+      <c r="A108" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="C108" s="22"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="10"/>
+      <c r="A109" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="C109" s="22"/>
     </row>
     <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C110" s="22"/>
+    </row>
+    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C111" s="22"/>
+    </row>
+    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="10"/>
+      <c r="C112" s="22"/>
+    </row>
+    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="10"/>
+      <c r="C113" s="22"/>
+    </row>
+    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C110" s="22"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
+      <c r="C114" s="22"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B111" s="9"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="9"/>
-      <c r="B112" s="9"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
+      <c r="B115" s="9"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A75:A80"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="A31:A37"/>
     <mergeCell ref="F1:L1"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A59:A67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="A2:A30"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A78:A85"/>
+    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="A60:A69"/>
+    <mergeCell ref="A2:A31"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="A32:A38"/>
   </mergeCells>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B28:B30" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If a list is required, enter each port on the same row in the next column to the right" sqref="B29:B31" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes if this subnet should be private, otherwise select No" sqref="B14:B17" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B31" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is the mount target name displayed in OCI console" sqref="B32" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22 E6:E7 E15:E17" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22 E6:E7 E15:E17 E85" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E14" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E38 E43" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>$A$99:$A$100</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E39 E44" xr:uid="{00000000-0002-0000-0000-000006000000}">
+      <formula1>$A$103:$A$104</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E39:E41 E44:E45" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E40:E42 E45:E46" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000008000000}">
-      <formula1>$A$110:$A$111</formula1>
+      <formula1>$A$114:$A$115</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E50:E51" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E51:E52" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>10</formula1>
       <formula2>4800</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E46" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="E47" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2902,7 +3003,7 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A99:A100 E38 E43" numberStoredAsText="1"/>
+    <ignoredError sqref="A103:A104 E39 E44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix for bug 116 - coh ports optional
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ADC43D-C795-4FD8-9927-1ECA1A0431B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF41D-02F4-449E-8A17-C6E5B12F2025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -721,15 +721,9 @@
     <t>Coherence cluster ports (leave blank if not used)</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence_cluster/port</t>
-  </si>
-  <si>
     <t>Coherence unicast ports (leave blank if not used)</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence_unicast/port</t>
-  </si>
-  <si>
     <t>Is this a SOA Domain? (e.g. it has any product of the SOA Suite like SOA, BPM, OSB or MFT)</t>
   </si>
   <si>
@@ -761,6 +755,12 @@
   </si>
   <si>
     <t xml:space="preserve">In the WLS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products mountpoint) </t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_cluster/opt</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_unicast/opt</t>
   </si>
 </sst>
 </file>
@@ -1242,24 +1242,24 @@
   </sheetPr>
   <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="128.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="128.7265625" customWidth="1"/>
+    <col min="3" max="3" width="44.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="48.1796875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
     </row>
-    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>13</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
         <v>61</v>
@@ -1315,7 +1315,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>63</v>
@@ -1330,7 +1330,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>83</v>
@@ -1345,7 +1345,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
         <v>67</v>
@@ -1360,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>43</v>
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>207</v>
@@ -1390,7 +1390,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
         <v>206</v>
@@ -1405,7 +1405,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>224</v>
@@ -1433,7 +1433,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>225</v>
@@ -1461,7 +1461,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>226</v>
@@ -1490,7 +1490,7 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>227</v>
@@ -1519,7 +1519,7 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>3</v>
@@ -1548,7 +1548,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -1577,7 +1577,7 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>5</v>
@@ -1606,7 +1606,7 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>6</v>
@@ -1635,7 +1635,7 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -1664,7 +1664,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1693,7 +1693,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>9</v>
@@ -1722,7 +1722,7 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>10</v>
@@ -1751,7 +1751,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
@@ -1780,7 +1780,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>16</v>
@@ -1809,7 +1809,7 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -1838,7 +1838,7 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>18</v>
@@ -1867,7 +1867,7 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
         <v>125</v>
@@ -1896,7 +1896,7 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
         <v>228</v>
@@ -1905,7 +1905,7 @@
         <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1925,16 +1925,16 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>165</v>
       </c>
       <c r="D28" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="E28">
         <v>8876</v>
@@ -1966,7 +1966,7 @@
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
         <v>19</v>
@@ -1993,7 +1993,7 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>211</v>
@@ -2005,7 +2005,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
       <c r="B31" s="5" t="s">
         <v>210</v>
@@ -2014,10 +2014,10 @@
         <v>204</v>
       </c>
       <c r="D31" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>24</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>26</v>
@@ -2049,7 +2049,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
         <v>27</v>
@@ -2064,7 +2064,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>72</v>
@@ -2079,7 +2079,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
         <v>28</v>
@@ -2094,7 +2094,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
         <v>29</v>
@@ -2109,7 +2109,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25"/>
       <c r="B38" s="5" t="s">
         <v>69</v>
@@ -2124,7 +2124,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>40</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
         <v>42</v>
@@ -2171,7 +2171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
         <v>65</v>
@@ -2186,7 +2186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
       <c r="B43" s="5" t="s">
         <v>64</v>
@@ -2201,7 +2201,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>174</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
         <v>87</v>
@@ -2233,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
         <v>88</v>
@@ -2248,7 +2248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
         <v>89</v>
@@ -2263,7 +2263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
         <v>90</v>
@@ -2278,7 +2278,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="25"/>
       <c r="B49" s="5" t="s">
         <v>119</v>
@@ -2293,7 +2293,7 @@
         <v>7777</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24" t="s">
         <v>111</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
         <v>116</v>
@@ -2325,7 +2325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
         <v>117</v>
@@ -2340,7 +2340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
         <v>222</v>
@@ -2355,7 +2355,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
         <v>123</v>
@@ -2367,7 +2367,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
         <v>223</v>
@@ -2382,7 +2382,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
         <v>160</v>
@@ -2394,7 +2394,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
         <v>120</v>
@@ -2409,7 +2409,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="24"/>
       <c r="B58" s="5" t="s">
         <v>118</v>
@@ -2424,7 +2424,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>92</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>93</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
         <v>194</v>
@@ -2473,7 +2473,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
         <v>190</v>
@@ -2488,7 +2488,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
         <v>193</v>
@@ -2503,7 +2503,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
         <v>149</v>
@@ -2521,7 +2521,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
         <v>171</v>
@@ -2536,7 +2536,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
         <v>169</v>
@@ -2551,7 +2551,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
         <v>172</v>
@@ -2566,7 +2566,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="24"/>
       <c r="B68" s="5" t="s">
         <v>177</v>
@@ -2581,24 +2581,24 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="24"/>
       <c r="B69" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C69" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="25" t="s">
         <v>182</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>165</v>
@@ -2610,10 +2610,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>165</v>
@@ -2625,10 +2625,10 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>165</v>
@@ -2640,10 +2640,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>165</v>
@@ -2655,7 +2655,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
         <v>94</v>
@@ -2673,7 +2673,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="25"/>
       <c r="B75" s="5" t="s">
         <v>150</v>
@@ -2688,7 +2688,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="25"/>
       <c r="B76" s="5" t="s">
         <v>152</v>
@@ -2703,19 +2703,19 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="25"/>
       <c r="B77" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C77" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="24" t="s">
         <v>178</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
         <v>219</v>
@@ -2741,7 +2741,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
         <v>218</v>
@@ -2753,7 +2753,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="24"/>
       <c r="B81" s="13" t="s">
         <v>217</v>
@@ -2765,7 +2765,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="24"/>
       <c r="B82" s="5" t="s">
         <v>221</v>
@@ -2777,7 +2777,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="24"/>
       <c r="B83" s="5" t="s">
         <v>216</v>
@@ -2789,7 +2789,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="24"/>
       <c r="B84" s="5" t="s">
         <v>215</v>
@@ -2801,22 +2801,22 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="24"/>
       <c r="B85" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C85" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D85" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E85" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>21</v>
       </c>
@@ -2825,132 +2825,132 @@
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="9"/>
     </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="11" t="s">
         <v>208</v>
       </c>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11" t="s">
         <v>209</v>
       </c>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="10"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="10"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B115" s="9"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
     </row>

</xml_diff>

<commit_message>
Fix for bug 116 - coh ports optional (#140)
</commit_message>
<xml_diff>
--- a/wls-hydr/sysconfig.xlsx
+++ b/wls-hydr/sysconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\repos\maa\wls-hydr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ADC43D-C795-4FD8-9927-1ECA1A0431B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF41D-02F4-449E-8A17-C6E5B12F2025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1680" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="virt_host_test" sheetId="1" r:id="rId1"/>
@@ -721,15 +721,9 @@
     <t>Coherence cluster ports (leave blank if not used)</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence_cluster/port</t>
-  </si>
-  <si>
     <t>Coherence unicast ports (leave blank if not used)</t>
   </si>
   <si>
-    <t>oci-network-ports-coherence_unicast/port</t>
-  </si>
-  <si>
     <t>Is this a SOA Domain? (e.g. it has any product of the SOA Suite like SOA, BPM, OSB or MFT)</t>
   </si>
   <si>
@@ -761,6 +755,12 @@
   </si>
   <si>
     <t xml:space="preserve">In the WLS nodes, the folder containing the JDK installation - leave blank if the JDK is under products (Products mountpoint) </t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_cluster/opt</t>
+  </si>
+  <si>
+    <t>oci-network-ports-coherence_unicast/opt</t>
   </si>
 </sst>
 </file>
@@ -1242,24 +1242,24 @@
   </sheetPr>
   <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="128.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="128.7265625" customWidth="1"/>
+    <col min="3" max="3" width="44.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="48.1796875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
     </row>
-    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>13</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
         <v>61</v>
@@ -1315,7 +1315,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>63</v>
@@ -1330,7 +1330,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>83</v>
@@ -1345,7 +1345,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
         <v>67</v>
@@ -1360,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>43</v>
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>207</v>
@@ -1390,7 +1390,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
         <v>206</v>
@@ -1405,7 +1405,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>224</v>
@@ -1433,7 +1433,7 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="5" t="s">
         <v>225</v>
@@ -1461,7 +1461,7 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>226</v>
@@ -1490,7 +1490,7 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>227</v>
@@ -1519,7 +1519,7 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>3</v>
@@ -1548,7 +1548,7 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -1577,7 +1577,7 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>5</v>
@@ -1606,7 +1606,7 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>6</v>
@@ -1635,7 +1635,7 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>7</v>
@@ -1664,7 +1664,7 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>8</v>
@@ -1693,7 +1693,7 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>9</v>
@@ -1722,7 +1722,7 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>10</v>
@@ -1751,7 +1751,7 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="5" t="s">
         <v>12</v>
@@ -1780,7 +1780,7 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>16</v>
@@ -1809,7 +1809,7 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -1838,7 +1838,7 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>18</v>
@@ -1867,7 +1867,7 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
         <v>125</v>
@@ -1896,7 +1896,7 @@
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
         <v>228</v>
@@ -1905,7 +1905,7 @@
         <v>165</v>
       </c>
       <c r="D27" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="E27">
         <v>7574</v>
@@ -1925,16 +1925,16 @@
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>165</v>
       </c>
       <c r="D28" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="E28">
         <v>8876</v>
@@ -1966,7 +1966,7 @@
       <c r="W28" s="6"/>
       <c r="X28" s="6"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="24"/>
       <c r="B29" s="5" t="s">
         <v>19</v>
@@ -1993,7 +1993,7 @@
         <v>9001</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="24"/>
       <c r="B30" s="5" t="s">
         <v>211</v>
@@ -2005,7 +2005,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="24"/>
       <c r="B31" s="5" t="s">
         <v>210</v>
@@ -2014,10 +2014,10 @@
         <v>204</v>
       </c>
       <c r="D31" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
         <v>24</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>26</v>
@@ -2049,7 +2049,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="25"/>
       <c r="B34" s="5" t="s">
         <v>27</v>
@@ -2064,7 +2064,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>72</v>
@@ -2079,7 +2079,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
         <v>28</v>
@@ -2094,7 +2094,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
         <v>29</v>
@@ -2109,7 +2109,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="25"/>
       <c r="B38" s="5" t="s">
         <v>69</v>
@@ -2124,7 +2124,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
         <v>40</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="24"/>
       <c r="B41" s="5" t="s">
         <v>42</v>
@@ -2171,7 +2171,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="24"/>
       <c r="B42" s="5" t="s">
         <v>65</v>
@@ -2186,7 +2186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
       <c r="B43" s="5" t="s">
         <v>64</v>
@@ -2201,7 +2201,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>174</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="25"/>
       <c r="B45" s="5" t="s">
         <v>87</v>
@@ -2233,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="25"/>
       <c r="B46" s="5" t="s">
         <v>88</v>
@@ -2248,7 +2248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="25"/>
       <c r="B47" s="5" t="s">
         <v>89</v>
@@ -2263,7 +2263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
         <v>90</v>
@@ -2278,7 +2278,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="25"/>
       <c r="B49" s="5" t="s">
         <v>119</v>
@@ -2293,7 +2293,7 @@
         <v>7777</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="24" t="s">
         <v>111</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
         <v>116</v>
@@ -2325,7 +2325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="24"/>
       <c r="B52" s="5" t="s">
         <v>117</v>
@@ -2340,7 +2340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="24"/>
       <c r="B53" s="5" t="s">
         <v>222</v>
@@ -2355,7 +2355,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="24"/>
       <c r="B54" s="5" t="s">
         <v>123</v>
@@ -2367,7 +2367,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="24"/>
       <c r="B55" s="5" t="s">
         <v>223</v>
@@ -2382,7 +2382,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="24"/>
       <c r="B56" s="5" t="s">
         <v>160</v>
@@ -2394,7 +2394,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="5" t="s">
         <v>120</v>
@@ -2409,7 +2409,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="24"/>
       <c r="B58" s="5" t="s">
         <v>118</v>
@@ -2424,7 +2424,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>92</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>93</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="24"/>
       <c r="B61" s="5" t="s">
         <v>194</v>
@@ -2473,7 +2473,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="24"/>
       <c r="B62" s="5" t="s">
         <v>190</v>
@@ -2488,7 +2488,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="24"/>
       <c r="B63" s="5" t="s">
         <v>193</v>
@@ -2503,7 +2503,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="24"/>
       <c r="B64" s="5" t="s">
         <v>149</v>
@@ -2521,7 +2521,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="24"/>
       <c r="B65" s="5" t="s">
         <v>171</v>
@@ -2536,7 +2536,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="24"/>
       <c r="B66" s="5" t="s">
         <v>169</v>
@@ -2551,7 +2551,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="24"/>
       <c r="B67" s="5" t="s">
         <v>172</v>
@@ -2566,7 +2566,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="24"/>
       <c r="B68" s="5" t="s">
         <v>177</v>
@@ -2581,24 +2581,24 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="24"/>
       <c r="B69" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C69" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="25" t="s">
         <v>182</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>165</v>
@@ -2610,10 +2610,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="25"/>
       <c r="B71" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>165</v>
@@ -2625,10 +2625,10 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="25"/>
       <c r="B72" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>165</v>
@@ -2640,10 +2640,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="25"/>
       <c r="B73" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>165</v>
@@ -2655,7 +2655,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="25"/>
       <c r="B74" s="5" t="s">
         <v>94</v>
@@ -2673,7 +2673,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="25"/>
       <c r="B75" s="5" t="s">
         <v>150</v>
@@ -2688,7 +2688,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="25"/>
       <c r="B76" s="5" t="s">
         <v>152</v>
@@ -2703,19 +2703,19 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="25"/>
       <c r="B77" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C77" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D77" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="24" t="s">
         <v>178</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="24"/>
       <c r="B79" s="5" t="s">
         <v>219</v>
@@ -2741,7 +2741,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="24"/>
       <c r="B80" s="5" t="s">
         <v>218</v>
@@ -2753,7 +2753,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="24"/>
       <c r="B81" s="13" t="s">
         <v>217</v>
@@ -2765,7 +2765,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="24"/>
       <c r="B82" s="5" t="s">
         <v>221</v>
@@ -2777,7 +2777,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="24"/>
       <c r="B83" s="5" t="s">
         <v>216</v>
@@ -2789,7 +2789,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="24"/>
       <c r="B84" s="5" t="s">
         <v>215</v>
@@ -2801,22 +2801,22 @@
         <v>214</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="24"/>
       <c r="B85" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C85" s="19" t="s">
         <v>204</v>
       </c>
       <c r="D85" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E85" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>21</v>
       </c>
@@ -2825,132 +2825,132 @@
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B97" s="9"/>
     </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="10"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="10"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="11" t="s">
         <v>208</v>
       </c>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11" t="s">
         <v>209</v>
       </c>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="10"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="10"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="10"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="10"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B115" s="9"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
     </row>

</xml_diff>